<commit_message>
Videos no youtube e codigo(chatgpt) para ligar esp32 a rede wifi e a um servidor onde coloca informação
</commit_message>
<xml_diff>
--- a/Diagrama Gant.xlsx
+++ b/Diagrama Gant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelabreu/Desktop/Smart metering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC4BD22-BC09-D74A-B71F-3818368FC814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FA9119-826D-8143-9528-F591D4B97FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{AC57B2E7-C3B7-485D-9028-5182123DD5F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{AC57B2E7-C3B7-485D-9028-5182123DD5F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="2" r:id="rId1"/>
@@ -292,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -315,43 +315,27 @@
     <xf numFmtId="16" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -361,14 +345,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,8 +423,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6243987" y="629052"/>
-          <a:ext cx="10990935" cy="1649568"/>
+          <a:off x="6252162" y="638862"/>
+          <a:ext cx="11268758" cy="1666851"/>
           <a:chOff x="6258249" y="639143"/>
           <a:chExt cx="11129982" cy="1664838"/>
         </a:xfrm>
@@ -1906,8 +1915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C326E24E-2340-7440-93FB-5CAF133542E1}">
   <dimension ref="B2:AU13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1919,160 +1928,160 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:47" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="12"/>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="12"/>
-      <c r="AI2" s="12"/>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="12"/>
-      <c r="AM2" s="12"/>
-      <c r="AN2" s="12"/>
-      <c r="AO2" s="12"/>
-      <c r="AP2" s="12"/>
-      <c r="AQ2" s="12"/>
-      <c r="AR2" s="12"/>
-      <c r="AS2" s="12"/>
-      <c r="AT2" s="18"/>
-      <c r="AU2" s="18"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23"/>
+      <c r="AE2" s="23"/>
+      <c r="AF2" s="23"/>
+      <c r="AG2" s="23"/>
+      <c r="AH2" s="23"/>
+      <c r="AI2" s="23"/>
+      <c r="AJ2" s="23"/>
+      <c r="AK2" s="23"/>
+      <c r="AL2" s="23"/>
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
+      <c r="AP2" s="23"/>
+      <c r="AQ2" s="23"/>
+      <c r="AR2" s="23"/>
+      <c r="AS2" s="23"/>
+      <c r="AT2" s="10"/>
+      <c r="AU2" s="10"/>
     </row>
     <row r="3" spans="2:47" x14ac:dyDescent="0.2">
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="17">
+      <c r="B3" s="26"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="24">
         <v>1</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17">
+      <c r="G3" s="24"/>
+      <c r="H3" s="24">
         <v>2</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="24">
         <v>2</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="24">
         <v>3</v>
       </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17">
+      <c r="K3" s="24"/>
+      <c r="L3" s="24">
         <v>4</v>
       </c>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17">
+      <c r="M3" s="24"/>
+      <c r="N3" s="24">
         <v>5</v>
       </c>
-      <c r="O3" s="17">
+      <c r="O3" s="24">
         <v>4</v>
       </c>
-      <c r="P3" s="17">
+      <c r="P3" s="24">
         <v>6</v>
       </c>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17">
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24">
         <v>7</v>
       </c>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17">
+      <c r="S3" s="24"/>
+      <c r="T3" s="24">
         <v>8</v>
       </c>
-      <c r="U3" s="17">
+      <c r="U3" s="24">
         <v>6</v>
       </c>
-      <c r="V3" s="17">
+      <c r="V3" s="24">
         <v>9</v>
       </c>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17">
+      <c r="W3" s="24"/>
+      <c r="X3" s="24">
         <v>10</v>
       </c>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17">
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24">
         <v>11</v>
       </c>
-      <c r="AA3" s="17">
+      <c r="AA3" s="24">
         <v>8</v>
       </c>
-      <c r="AB3" s="17">
+      <c r="AB3" s="24">
         <v>12</v>
       </c>
-      <c r="AC3" s="17"/>
-      <c r="AD3" s="17">
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24">
         <v>13</v>
       </c>
-      <c r="AE3" s="17"/>
-      <c r="AF3" s="17">
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24">
         <v>14</v>
       </c>
-      <c r="AG3" s="17">
+      <c r="AG3" s="24">
         <v>10</v>
       </c>
-      <c r="AH3" s="17">
+      <c r="AH3" s="24">
         <v>15</v>
       </c>
-      <c r="AI3" s="17"/>
-      <c r="AJ3" s="17">
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="24">
         <v>16</v>
       </c>
-      <c r="AK3" s="17"/>
-      <c r="AL3" s="17">
+      <c r="AK3" s="24"/>
+      <c r="AL3" s="24">
         <v>17</v>
       </c>
-      <c r="AM3" s="17"/>
-      <c r="AN3" s="17">
+      <c r="AM3" s="24"/>
+      <c r="AN3" s="24">
         <v>18</v>
       </c>
-      <c r="AO3" s="17"/>
-      <c r="AP3" s="17">
+      <c r="AO3" s="24"/>
+      <c r="AP3" s="24">
         <v>19</v>
       </c>
-      <c r="AQ3" s="17"/>
-      <c r="AR3" s="17">
+      <c r="AQ3" s="24"/>
+      <c r="AR3" s="24">
         <v>20</v>
       </c>
-      <c r="AS3" s="17"/>
-      <c r="AT3" s="18"/>
-      <c r="AU3" s="18"/>
+      <c r="AS3" s="24"/>
+      <c r="AT3" s="10"/>
+      <c r="AU3" s="10"/>
     </row>
     <row r="4" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
@@ -2085,48 +2094,48 @@
         <v>44989</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="25"/>
-      <c r="AD4" s="25"/>
-      <c r="AE4" s="25"/>
-      <c r="AF4" s="25"/>
-      <c r="AG4" s="25"/>
-      <c r="AH4" s="25"/>
-      <c r="AI4" s="25"/>
-      <c r="AJ4" s="25"/>
-      <c r="AK4" s="25"/>
-      <c r="AL4" s="25"/>
-      <c r="AM4" s="25"/>
-      <c r="AN4" s="25"/>
-      <c r="AO4" s="25"/>
-      <c r="AP4" s="25"/>
-      <c r="AQ4" s="25"/>
-      <c r="AR4" s="25"/>
-      <c r="AS4" s="25"/>
-      <c r="AT4" s="18"/>
-      <c r="AU4" s="18"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="22"/>
+      <c r="AH4" s="22"/>
+      <c r="AI4" s="22"/>
+      <c r="AJ4" s="22"/>
+      <c r="AK4" s="22"/>
+      <c r="AL4" s="22"/>
+      <c r="AM4" s="22"/>
+      <c r="AN4" s="22"/>
+      <c r="AO4" s="22"/>
+      <c r="AP4" s="22"/>
+      <c r="AQ4" s="22"/>
+      <c r="AR4" s="22"/>
+      <c r="AS4" s="22"/>
+      <c r="AT4" s="10"/>
+      <c r="AU4" s="10"/>
     </row>
     <row r="5" spans="2:47" ht="32" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
@@ -2139,48 +2148,48 @@
         <v>44996</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="25"/>
-      <c r="W5" s="25"/>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="25"/>
-      <c r="Z5" s="25"/>
-      <c r="AA5" s="25"/>
-      <c r="AB5" s="25"/>
-      <c r="AC5" s="25"/>
-      <c r="AD5" s="25"/>
-      <c r="AE5" s="25"/>
-      <c r="AF5" s="25"/>
-      <c r="AG5" s="25"/>
-      <c r="AH5" s="25"/>
-      <c r="AI5" s="25"/>
-      <c r="AJ5" s="25"/>
-      <c r="AK5" s="25"/>
-      <c r="AL5" s="25"/>
-      <c r="AM5" s="25"/>
-      <c r="AN5" s="25"/>
-      <c r="AO5" s="25"/>
-      <c r="AP5" s="25"/>
-      <c r="AQ5" s="25"/>
-      <c r="AR5" s="25"/>
-      <c r="AS5" s="25"/>
-      <c r="AT5" s="18"/>
-      <c r="AU5" s="18"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="22"/>
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="22"/>
+      <c r="AD5" s="22"/>
+      <c r="AE5" s="22"/>
+      <c r="AF5" s="22"/>
+      <c r="AG5" s="22"/>
+      <c r="AH5" s="22"/>
+      <c r="AI5" s="22"/>
+      <c r="AJ5" s="22"/>
+      <c r="AK5" s="22"/>
+      <c r="AL5" s="22"/>
+      <c r="AM5" s="22"/>
+      <c r="AN5" s="22"/>
+      <c r="AO5" s="22"/>
+      <c r="AP5" s="22"/>
+      <c r="AQ5" s="22"/>
+      <c r="AR5" s="22"/>
+      <c r="AS5" s="22"/>
+      <c r="AT5" s="10"/>
+      <c r="AU5" s="10"/>
     </row>
     <row r="6" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -2193,48 +2202,48 @@
         <v>45031</v>
       </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="25"/>
-      <c r="Y6" s="25"/>
-      <c r="Z6" s="25"/>
-      <c r="AA6" s="25"/>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="25"/>
-      <c r="AD6" s="25"/>
-      <c r="AE6" s="25"/>
-      <c r="AF6" s="25"/>
-      <c r="AG6" s="25"/>
-      <c r="AH6" s="25"/>
-      <c r="AI6" s="25"/>
-      <c r="AJ6" s="25"/>
-      <c r="AK6" s="25"/>
-      <c r="AL6" s="25"/>
-      <c r="AM6" s="25"/>
-      <c r="AN6" s="25"/>
-      <c r="AO6" s="25"/>
-      <c r="AP6" s="25"/>
-      <c r="AQ6" s="25"/>
-      <c r="AR6" s="25"/>
-      <c r="AS6" s="25"/>
-      <c r="AT6" s="18"/>
-      <c r="AU6" s="18"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="22"/>
+      <c r="AF6" s="22"/>
+      <c r="AG6" s="22"/>
+      <c r="AH6" s="22"/>
+      <c r="AI6" s="22"/>
+      <c r="AJ6" s="22"/>
+      <c r="AK6" s="22"/>
+      <c r="AL6" s="22"/>
+      <c r="AM6" s="22"/>
+      <c r="AN6" s="22"/>
+      <c r="AO6" s="22"/>
+      <c r="AP6" s="22"/>
+      <c r="AQ6" s="22"/>
+      <c r="AR6" s="22"/>
+      <c r="AS6" s="22"/>
+      <c r="AT6" s="10"/>
+      <c r="AU6" s="10"/>
     </row>
     <row r="7" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
@@ -2247,102 +2256,102 @@
         <v>45031</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="25"/>
-      <c r="W7" s="25"/>
-      <c r="X7" s="25"/>
-      <c r="Y7" s="25"/>
-      <c r="Z7" s="25"/>
-      <c r="AA7" s="25"/>
-      <c r="AB7" s="25"/>
-      <c r="AC7" s="25"/>
-      <c r="AD7" s="25"/>
-      <c r="AE7" s="25"/>
-      <c r="AF7" s="25"/>
-      <c r="AG7" s="25"/>
-      <c r="AH7" s="25"/>
-      <c r="AI7" s="25"/>
-      <c r="AJ7" s="25"/>
-      <c r="AK7" s="25"/>
-      <c r="AL7" s="25"/>
-      <c r="AM7" s="25"/>
-      <c r="AN7" s="25"/>
-      <c r="AO7" s="25"/>
-      <c r="AP7" s="25"/>
-      <c r="AQ7" s="25"/>
-      <c r="AR7" s="25"/>
-      <c r="AS7" s="25"/>
-      <c r="AT7" s="18"/>
-      <c r="AU7" s="18"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
+      <c r="Z7" s="22"/>
+      <c r="AA7" s="22"/>
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="22"/>
+      <c r="AD7" s="22"/>
+      <c r="AE7" s="22"/>
+      <c r="AF7" s="22"/>
+      <c r="AG7" s="22"/>
+      <c r="AH7" s="22"/>
+      <c r="AI7" s="22"/>
+      <c r="AJ7" s="22"/>
+      <c r="AK7" s="22"/>
+      <c r="AL7" s="22"/>
+      <c r="AM7" s="22"/>
+      <c r="AN7" s="22"/>
+      <c r="AO7" s="22"/>
+      <c r="AP7" s="22"/>
+      <c r="AQ7" s="22"/>
+      <c r="AR7" s="22"/>
+      <c r="AS7" s="22"/>
+      <c r="AT7" s="10"/>
+      <c r="AU7" s="10"/>
     </row>
     <row r="8" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="9">
         <v>45032</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="9">
         <v>45059</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="25"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="25"/>
-      <c r="X8" s="25"/>
-      <c r="Y8" s="25"/>
-      <c r="Z8" s="25"/>
-      <c r="AA8" s="25"/>
-      <c r="AB8" s="25"/>
-      <c r="AC8" s="25"/>
-      <c r="AD8" s="25"/>
-      <c r="AE8" s="25"/>
-      <c r="AF8" s="25"/>
-      <c r="AG8" s="25"/>
-      <c r="AH8" s="25"/>
-      <c r="AI8" s="25"/>
-      <c r="AJ8" s="25"/>
-      <c r="AK8" s="25"/>
-      <c r="AL8" s="25"/>
-      <c r="AM8" s="25"/>
-      <c r="AN8" s="25"/>
-      <c r="AO8" s="25"/>
-      <c r="AP8" s="25"/>
-      <c r="AQ8" s="25"/>
-      <c r="AR8" s="25"/>
-      <c r="AS8" s="25"/>
-      <c r="AT8" s="18"/>
-      <c r="AU8" s="18"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="22"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="22"/>
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22"/>
+      <c r="AE8" s="22"/>
+      <c r="AF8" s="22"/>
+      <c r="AG8" s="22"/>
+      <c r="AH8" s="22"/>
+      <c r="AI8" s="22"/>
+      <c r="AJ8" s="22"/>
+      <c r="AK8" s="22"/>
+      <c r="AL8" s="22"/>
+      <c r="AM8" s="22"/>
+      <c r="AN8" s="22"/>
+      <c r="AO8" s="22"/>
+      <c r="AP8" s="22"/>
+      <c r="AQ8" s="22"/>
+      <c r="AR8" s="22"/>
+      <c r="AS8" s="22"/>
+      <c r="AT8" s="10"/>
+      <c r="AU8" s="10"/>
     </row>
     <row r="9" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
@@ -2355,48 +2364,48 @@
         <v>45084</v>
       </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="25"/>
-      <c r="W9" s="25"/>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="25"/>
-      <c r="Z9" s="25"/>
-      <c r="AA9" s="25"/>
-      <c r="AB9" s="25"/>
-      <c r="AC9" s="25"/>
-      <c r="AD9" s="25"/>
-      <c r="AE9" s="25"/>
-      <c r="AF9" s="25"/>
-      <c r="AG9" s="25"/>
-      <c r="AH9" s="25"/>
-      <c r="AI9" s="25"/>
-      <c r="AJ9" s="25"/>
-      <c r="AK9" s="25"/>
-      <c r="AL9" s="25"/>
-      <c r="AM9" s="25"/>
-      <c r="AN9" s="25"/>
-      <c r="AO9" s="25"/>
-      <c r="AP9" s="25"/>
-      <c r="AQ9" s="25"/>
-      <c r="AR9" s="25"/>
-      <c r="AS9" s="25"/>
-      <c r="AT9" s="18"/>
-      <c r="AU9" s="18"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22"/>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="22"/>
+      <c r="AH9" s="22"/>
+      <c r="AI9" s="22"/>
+      <c r="AJ9" s="22"/>
+      <c r="AK9" s="22"/>
+      <c r="AL9" s="22"/>
+      <c r="AM9" s="22"/>
+      <c r="AN9" s="22"/>
+      <c r="AO9" s="22"/>
+      <c r="AP9" s="22"/>
+      <c r="AQ9" s="22"/>
+      <c r="AR9" s="22"/>
+      <c r="AS9" s="22"/>
+      <c r="AT9" s="10"/>
+      <c r="AU9" s="10"/>
     </row>
     <row r="10" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
@@ -2408,49 +2417,49 @@
       <c r="D10" s="4">
         <v>45087</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="25"/>
-      <c r="Y10" s="25"/>
-      <c r="Z10" s="25"/>
-      <c r="AA10" s="25"/>
-      <c r="AB10" s="25"/>
-      <c r="AC10" s="25"/>
-      <c r="AD10" s="25"/>
-      <c r="AE10" s="25"/>
-      <c r="AF10" s="25"/>
-      <c r="AG10" s="25"/>
-      <c r="AH10" s="25"/>
-      <c r="AI10" s="25"/>
-      <c r="AJ10" s="25"/>
-      <c r="AK10" s="25"/>
-      <c r="AL10" s="25"/>
-      <c r="AM10" s="25"/>
-      <c r="AN10" s="25"/>
-      <c r="AO10" s="25"/>
-      <c r="AP10" s="25"/>
-      <c r="AQ10" s="25"/>
-      <c r="AR10" s="25"/>
-      <c r="AS10" s="25"/>
-      <c r="AT10" s="18"/>
-      <c r="AU10" s="18"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22"/>
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="22"/>
+      <c r="AE10" s="22"/>
+      <c r="AF10" s="22"/>
+      <c r="AG10" s="22"/>
+      <c r="AH10" s="22"/>
+      <c r="AI10" s="22"/>
+      <c r="AJ10" s="22"/>
+      <c r="AK10" s="22"/>
+      <c r="AL10" s="22"/>
+      <c r="AM10" s="22"/>
+      <c r="AN10" s="22"/>
+      <c r="AO10" s="22"/>
+      <c r="AP10" s="22"/>
+      <c r="AQ10" s="22"/>
+      <c r="AR10" s="22"/>
+      <c r="AS10" s="22"/>
+      <c r="AT10" s="10"/>
+      <c r="AU10" s="10"/>
     </row>
     <row r="11" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
@@ -2462,240 +2471,406 @@
       <c r="D11" s="4">
         <v>45101</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="25"/>
-      <c r="V11" s="25"/>
-      <c r="W11" s="25"/>
-      <c r="X11" s="25"/>
-      <c r="Y11" s="25"/>
-      <c r="Z11" s="25"/>
-      <c r="AA11" s="25"/>
-      <c r="AB11" s="25"/>
-      <c r="AC11" s="25"/>
-      <c r="AD11" s="25"/>
-      <c r="AE11" s="25"/>
-      <c r="AF11" s="25"/>
-      <c r="AG11" s="25"/>
-      <c r="AH11" s="25"/>
-      <c r="AI11" s="25"/>
-      <c r="AJ11" s="25"/>
-      <c r="AK11" s="25"/>
-      <c r="AL11" s="25"/>
-      <c r="AM11" s="25"/>
-      <c r="AN11" s="25"/>
-      <c r="AO11" s="25"/>
-      <c r="AP11" s="25"/>
-      <c r="AQ11" s="25"/>
-      <c r="AR11" s="25"/>
-      <c r="AS11" s="25"/>
-      <c r="AT11" s="18"/>
-      <c r="AU11" s="18"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="22"/>
+      <c r="Z11" s="22"/>
+      <c r="AA11" s="22"/>
+      <c r="AB11" s="22"/>
+      <c r="AC11" s="22"/>
+      <c r="AD11" s="22"/>
+      <c r="AE11" s="22"/>
+      <c r="AF11" s="22"/>
+      <c r="AG11" s="22"/>
+      <c r="AH11" s="22"/>
+      <c r="AI11" s="22"/>
+      <c r="AJ11" s="22"/>
+      <c r="AK11" s="22"/>
+      <c r="AL11" s="22"/>
+      <c r="AM11" s="22"/>
+      <c r="AN11" s="22"/>
+      <c r="AO11" s="22"/>
+      <c r="AP11" s="22"/>
+      <c r="AQ11" s="22"/>
+      <c r="AR11" s="22"/>
+      <c r="AS11" s="22"/>
+      <c r="AT11" s="10"/>
+      <c r="AU11" s="10"/>
     </row>
     <row r="12" spans="2:47" x14ac:dyDescent="0.2">
-      <c r="B12" s="26"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="2" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="12">
         <v>5</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="13">
         <v>11</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="12">
         <v>12</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="13">
         <v>18</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="12">
         <v>19</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="13">
         <v>25</v>
       </c>
-      <c r="L12" s="19">
+      <c r="L12" s="12">
         <v>26</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M12" s="13">
         <v>4</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="12">
         <v>5</v>
       </c>
-      <c r="O12" s="19">
+      <c r="O12" s="13">
         <v>11</v>
       </c>
-      <c r="P12" s="19">
+      <c r="P12" s="12">
         <v>12</v>
       </c>
-      <c r="Q12" s="19">
+      <c r="Q12" s="13">
         <v>18</v>
       </c>
-      <c r="R12" s="19">
+      <c r="R12" s="12">
         <v>19</v>
       </c>
-      <c r="S12" s="19">
+      <c r="S12" s="13">
         <v>25</v>
       </c>
-      <c r="T12" s="19">
+      <c r="T12" s="12">
         <v>26</v>
       </c>
-      <c r="U12" s="19">
+      <c r="U12" s="13">
         <v>1</v>
       </c>
-      <c r="V12" s="19">
+      <c r="V12" s="12">
         <v>2</v>
       </c>
-      <c r="W12" s="19">
+      <c r="W12" s="13">
         <v>8</v>
       </c>
-      <c r="X12" s="19">
+      <c r="X12" s="12">
         <v>9</v>
       </c>
-      <c r="Y12" s="19">
+      <c r="Y12" s="13">
         <v>15</v>
       </c>
-      <c r="Z12" s="19">
+      <c r="Z12" s="12">
         <v>16</v>
       </c>
-      <c r="AA12" s="19">
+      <c r="AA12" s="13">
         <v>22</v>
       </c>
-      <c r="AB12" s="19">
+      <c r="AB12" s="12">
         <v>23</v>
       </c>
-      <c r="AC12" s="19">
+      <c r="AC12" s="13">
         <v>29</v>
       </c>
-      <c r="AD12" s="19">
+      <c r="AD12" s="12">
         <v>30</v>
       </c>
-      <c r="AE12" s="19">
+      <c r="AE12" s="13">
         <v>6</v>
       </c>
-      <c r="AF12" s="19">
+      <c r="AF12" s="12">
         <v>7</v>
       </c>
-      <c r="AG12" s="19">
+      <c r="AG12" s="13">
         <v>13</v>
       </c>
-      <c r="AH12" s="19">
+      <c r="AH12" s="12">
         <v>14</v>
       </c>
-      <c r="AI12" s="19">
+      <c r="AI12" s="13">
         <v>20</v>
       </c>
-      <c r="AJ12" s="19">
+      <c r="AJ12" s="12">
         <v>21</v>
       </c>
-      <c r="AK12" s="19">
+      <c r="AK12" s="13">
         <v>27</v>
       </c>
-      <c r="AL12" s="19">
+      <c r="AL12" s="12">
         <v>28</v>
       </c>
-      <c r="AM12" s="19">
+      <c r="AM12" s="13">
         <v>3</v>
       </c>
-      <c r="AN12" s="19">
+      <c r="AN12" s="12">
         <v>4</v>
       </c>
-      <c r="AO12" s="19">
+      <c r="AO12" s="13">
         <v>10</v>
       </c>
-      <c r="AP12" s="19">
+      <c r="AP12" s="12">
         <v>11</v>
       </c>
-      <c r="AQ12" s="19">
+      <c r="AQ12" s="13">
         <v>17</v>
       </c>
-      <c r="AR12" s="19">
+      <c r="AR12" s="12">
         <v>18</v>
       </c>
-      <c r="AS12" s="19">
+      <c r="AS12" s="13">
         <v>24</v>
       </c>
-      <c r="AT12" s="18"/>
-      <c r="AU12" s="18"/>
+      <c r="AT12" s="10"/>
+      <c r="AU12" s="10"/>
     </row>
     <row r="13" spans="2:47" x14ac:dyDescent="0.2">
-      <c r="B13" s="20"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="29"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="18"/>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="19">
         <v>2</v>
       </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="21">
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="19">
         <v>3</v>
       </c>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="22"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="21">
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="19">
         <v>4</v>
       </c>
-      <c r="V13" s="22"/>
-      <c r="W13" s="22"/>
-      <c r="X13" s="22"/>
-      <c r="Y13" s="22"/>
-      <c r="Z13" s="22"/>
-      <c r="AA13" s="22"/>
-      <c r="AB13" s="22"/>
-      <c r="AC13" s="22"/>
-      <c r="AD13" s="23"/>
-      <c r="AE13" s="21">
+      <c r="V13" s="20"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="20"/>
+      <c r="Z13" s="20"/>
+      <c r="AA13" s="20"/>
+      <c r="AB13" s="20"/>
+      <c r="AC13" s="20"/>
+      <c r="AD13" s="21"/>
+      <c r="AE13" s="19">
         <v>5</v>
       </c>
-      <c r="AF13" s="22"/>
-      <c r="AG13" s="22"/>
-      <c r="AH13" s="22"/>
-      <c r="AI13" s="22"/>
-      <c r="AJ13" s="22"/>
-      <c r="AK13" s="22"/>
-      <c r="AL13" s="23"/>
-      <c r="AM13" s="21">
+      <c r="AF13" s="20"/>
+      <c r="AG13" s="20"/>
+      <c r="AH13" s="20"/>
+      <c r="AI13" s="20"/>
+      <c r="AJ13" s="20"/>
+      <c r="AK13" s="20"/>
+      <c r="AL13" s="21"/>
+      <c r="AM13" s="19">
         <v>6</v>
       </c>
-      <c r="AN13" s="22"/>
-      <c r="AO13" s="22"/>
-      <c r="AP13" s="22"/>
-      <c r="AQ13" s="22"/>
-      <c r="AR13" s="22"/>
-      <c r="AS13" s="23"/>
+      <c r="AN13" s="20"/>
+      <c r="AO13" s="20"/>
+      <c r="AP13" s="20"/>
+      <c r="AQ13" s="20"/>
+      <c r="AR13" s="20"/>
+      <c r="AS13" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="190">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AR3:AS3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AP4:AQ4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="AD4:AE4"/>
+    <mergeCell ref="AF4:AG4"/>
+    <mergeCell ref="AH4:AI4"/>
+    <mergeCell ref="AJ4:AK4"/>
+    <mergeCell ref="AL4:AM4"/>
+    <mergeCell ref="AN4:AO4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="AR5:AS5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="AL5:AM5"/>
+    <mergeCell ref="AN5:AO5"/>
+    <mergeCell ref="AP5:AQ5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AH6:AI6"/>
+    <mergeCell ref="AJ6:AK6"/>
+    <mergeCell ref="AL6:AM6"/>
+    <mergeCell ref="AN6:AO6"/>
+    <mergeCell ref="AP6:AQ6"/>
+    <mergeCell ref="AR6:AS6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="AF6:AG6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="AJ7:AK7"/>
+    <mergeCell ref="AL7:AM7"/>
+    <mergeCell ref="AN7:AO7"/>
+    <mergeCell ref="AP7:AQ7"/>
+    <mergeCell ref="AR7:AS7"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="AF7:AG7"/>
+    <mergeCell ref="AH7:AI7"/>
+    <mergeCell ref="AP8:AQ8"/>
+    <mergeCell ref="AR8:AS8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="AD8:AE8"/>
+    <mergeCell ref="AF8:AG8"/>
+    <mergeCell ref="AH8:AI8"/>
+    <mergeCell ref="AJ8:AK8"/>
+    <mergeCell ref="AL8:AM8"/>
+    <mergeCell ref="AN8:AO8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="AR9:AS9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="T10:U10"/>
+    <mergeCell ref="AF9:AG9"/>
+    <mergeCell ref="AH9:AI9"/>
+    <mergeCell ref="AJ9:AK9"/>
+    <mergeCell ref="AL9:AM9"/>
+    <mergeCell ref="AN9:AO9"/>
+    <mergeCell ref="AP9:AQ9"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="Z9:AA9"/>
+    <mergeCell ref="AB9:AC9"/>
+    <mergeCell ref="AD9:AE9"/>
+    <mergeCell ref="AF11:AG11"/>
+    <mergeCell ref="AH11:AI11"/>
+    <mergeCell ref="AH10:AI10"/>
+    <mergeCell ref="AJ10:AK10"/>
+    <mergeCell ref="AL10:AM10"/>
+    <mergeCell ref="AN10:AO10"/>
+    <mergeCell ref="AP10:AQ10"/>
+    <mergeCell ref="AR10:AS10"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="X10:Y10"/>
+    <mergeCell ref="Z10:AA10"/>
+    <mergeCell ref="AB10:AC10"/>
+    <mergeCell ref="AD10:AE10"/>
+    <mergeCell ref="AF10:AG10"/>
     <mergeCell ref="AM13:AS13"/>
     <mergeCell ref="T11:U11"/>
     <mergeCell ref="V11:W11"/>
@@ -2720,172 +2895,6 @@
     <mergeCell ref="Z11:AA11"/>
     <mergeCell ref="AB11:AC11"/>
     <mergeCell ref="AD11:AE11"/>
-    <mergeCell ref="AF11:AG11"/>
-    <mergeCell ref="AH11:AI11"/>
-    <mergeCell ref="AH10:AI10"/>
-    <mergeCell ref="AJ10:AK10"/>
-    <mergeCell ref="AL10:AM10"/>
-    <mergeCell ref="AN10:AO10"/>
-    <mergeCell ref="AP10:AQ10"/>
-    <mergeCell ref="AR10:AS10"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="X10:Y10"/>
-    <mergeCell ref="Z10:AA10"/>
-    <mergeCell ref="AB10:AC10"/>
-    <mergeCell ref="AD10:AE10"/>
-    <mergeCell ref="AF10:AG10"/>
-    <mergeCell ref="AR9:AS9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="T10:U10"/>
-    <mergeCell ref="AF9:AG9"/>
-    <mergeCell ref="AH9:AI9"/>
-    <mergeCell ref="AJ9:AK9"/>
-    <mergeCell ref="AL9:AM9"/>
-    <mergeCell ref="AN9:AO9"/>
-    <mergeCell ref="AP9:AQ9"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="X9:Y9"/>
-    <mergeCell ref="Z9:AA9"/>
-    <mergeCell ref="AB9:AC9"/>
-    <mergeCell ref="AD9:AE9"/>
-    <mergeCell ref="AP8:AQ8"/>
-    <mergeCell ref="AR8:AS8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="AD8:AE8"/>
-    <mergeCell ref="AF8:AG8"/>
-    <mergeCell ref="AH8:AI8"/>
-    <mergeCell ref="AJ8:AK8"/>
-    <mergeCell ref="AL8:AM8"/>
-    <mergeCell ref="AN8:AO8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="Z8:AA8"/>
-    <mergeCell ref="AB8:AC8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="AJ7:AK7"/>
-    <mergeCell ref="AL7:AM7"/>
-    <mergeCell ref="AN7:AO7"/>
-    <mergeCell ref="AP7:AQ7"/>
-    <mergeCell ref="AR7:AS7"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="AD7:AE7"/>
-    <mergeCell ref="AF7:AG7"/>
-    <mergeCell ref="AH7:AI7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="AH6:AI6"/>
-    <mergeCell ref="AJ6:AK6"/>
-    <mergeCell ref="AL6:AM6"/>
-    <mergeCell ref="AN6:AO6"/>
-    <mergeCell ref="AP6:AQ6"/>
-    <mergeCell ref="AR6:AS6"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="AF6:AG6"/>
-    <mergeCell ref="AR5:AS5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="AH5:AI5"/>
-    <mergeCell ref="AJ5:AK5"/>
-    <mergeCell ref="AL5:AM5"/>
-    <mergeCell ref="AN5:AO5"/>
-    <mergeCell ref="AP5:AQ5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="AP4:AQ4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="AD4:AE4"/>
-    <mergeCell ref="AF4:AG4"/>
-    <mergeCell ref="AH4:AI4"/>
-    <mergeCell ref="AJ4:AK4"/>
-    <mergeCell ref="AL4:AM4"/>
-    <mergeCell ref="AN4:AO4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:Y4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="AR3:AS3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F11 H5:H11 J5:J11 L5:L11 N5:N11 P5:P11 R5:R11 T5:T11 V5:V11 X5:X11 Z5:Z11 AB5:AB11 AD5:AD11 AF5:AF11 AH5:AH11 AJ5:AJ11 AL5:AL11">
     <cfRule type="dataBar" priority="2">

</xml_diff>

<commit_message>
Finalização gantt Inicio budget
</commit_message>
<xml_diff>
--- a/Diagrama Gant.xlsx
+++ b/Diagrama Gant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelabreu/Desktop/Smart metering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8611099C-6370-EC4A-9ECF-3DE4A316AF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFA3975-AAF9-0A4C-B949-CC6D5193A198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{AC57B2E7-C3B7-485D-9028-5182123DD5F2}"/>
   </bookViews>
@@ -94,9 +94,6 @@
     <t>Final technical report</t>
   </si>
   <si>
-    <t>Ligar ESP32 ao WiFi e conectar os Relés (incluindo trabalho de software)</t>
-  </si>
-  <si>
     <t>Sensor Temperatura e LED (incluindo trabalho de software )</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>LCD e Botão (incluindo trabalho de software)</t>
+  </si>
+  <si>
+    <t>Ligar ESP32 ao WiFi e conectar os Relés (incluindo trabalho de software, tal como conexão a app HOME e ao servidor)</t>
   </si>
 </sst>
 </file>
@@ -367,6 +367,21 @@
     <xf numFmtId="16" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -392,22 +407,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,8 +454,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6293443" y="625314"/>
-          <a:ext cx="11035009" cy="3496849"/>
+          <a:off x="6292327" y="639968"/>
+          <a:ext cx="11024123" cy="3735776"/>
           <a:chOff x="6277776" y="614399"/>
           <a:chExt cx="11006428" cy="2652949"/>
         </a:xfrm>
@@ -648,9 +648,9 @@
         <xdr:grpSpPr>
           <a:xfrm>
             <a:off x="8493346" y="917411"/>
-            <a:ext cx="3227526" cy="502274"/>
+            <a:ext cx="3227526" cy="532911"/>
             <a:chOff x="8493346" y="917411"/>
-            <a:chExt cx="3227526" cy="502274"/>
+            <a:chExt cx="3227526" cy="532911"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:grpSp>
@@ -686,7 +686,7 @@
             <xdr:spPr>
               <a:xfrm>
                 <a:off x="8515133" y="898556"/>
-                <a:ext cx="455823" cy="215678"/>
+                <a:ext cx="455823" cy="187934"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
                 <a:avLst/>
@@ -839,7 +839,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="8994904" y="1257881"/>
-              <a:ext cx="2725968" cy="161804"/>
+              <a:ext cx="2725968" cy="192441"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -890,9 +890,9 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="15510091" y="2753654"/>
+            <a:off x="15510091" y="2775250"/>
             <a:ext cx="687533" cy="223465"/>
-            <a:chOff x="15510091" y="2753654"/>
+            <a:chOff x="15510091" y="2775250"/>
             <a:chExt cx="687533" cy="223465"/>
           </a:xfrm>
         </xdr:grpSpPr>
@@ -909,7 +909,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="15698272" y="2889572"/>
+              <a:off x="15698272" y="2911168"/>
               <a:ext cx="499352" cy="87547"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -960,10 +960,10 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="15510091" y="2753654"/>
-              <a:ext cx="178656" cy="181048"/>
-              <a:chOff x="15562495" y="2362333"/>
-              <a:chExt cx="179436" cy="184857"/>
+              <a:off x="15510091" y="2775250"/>
+              <a:ext cx="178656" cy="181049"/>
+              <a:chOff x="15562495" y="2384381"/>
+              <a:chExt cx="179436" cy="184858"/>
             </a:xfrm>
           </xdr:grpSpPr>
           <xdr:cxnSp macro="">
@@ -979,7 +979,7 @@
             </xdr:nvCxnSpPr>
             <xdr:spPr>
               <a:xfrm>
-                <a:off x="15562495" y="2543750"/>
+                <a:off x="15562495" y="2565799"/>
                 <a:ext cx="179436" cy="3440"/>
               </a:xfrm>
               <a:prstGeom prst="straightConnector1">
@@ -1020,7 +1020,7 @@
             </xdr:nvCxnSpPr>
             <xdr:spPr>
               <a:xfrm flipH="1">
-                <a:off x="15562495" y="2362333"/>
+                <a:off x="15562495" y="2384381"/>
                 <a:ext cx="1796" cy="184695"/>
               </a:xfrm>
               <a:prstGeom prst="line">
@@ -1063,9 +1063,9 @@
         <xdr:grpSpPr>
           <a:xfrm>
             <a:off x="7899928" y="754150"/>
-            <a:ext cx="780083" cy="291739"/>
+            <a:ext cx="780083" cy="255315"/>
             <a:chOff x="7905917" y="754230"/>
-            <a:chExt cx="499949" cy="299973"/>
+            <a:chExt cx="499949" cy="262521"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
@@ -1132,7 +1132,7 @@
           </xdr:nvCxnSpPr>
           <xdr:spPr>
             <a:xfrm flipV="1">
-              <a:off x="8156140" y="1051692"/>
+              <a:off x="8156140" y="1014240"/>
               <a:ext cx="129234" cy="1940"/>
             </a:xfrm>
             <a:prstGeom prst="straightConnector1">
@@ -1169,13 +1169,11 @@
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
-            <xdr:cNvCxnSpPr>
-              <a:stCxn id="5" idx="2"/>
-            </xdr:cNvCxnSpPr>
+            <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
             <a:xfrm flipH="1">
-              <a:off x="8155621" y="857579"/>
+              <a:off x="8155621" y="820127"/>
               <a:ext cx="271" cy="196624"/>
             </a:xfrm>
             <a:prstGeom prst="line">
@@ -1216,10 +1214,10 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="10734216" y="1572308"/>
-            <a:ext cx="984762" cy="295852"/>
-            <a:chOff x="10734216" y="1572308"/>
-            <a:chExt cx="984762" cy="295852"/>
+            <a:off x="10734216" y="1642483"/>
+            <a:ext cx="984762" cy="295857"/>
+            <a:chOff x="10734216" y="1642483"/>
+            <a:chExt cx="984762" cy="295857"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
@@ -1235,7 +1233,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10983795" y="1694713"/>
+              <a:off x="10983795" y="1764893"/>
               <a:ext cx="735183" cy="173447"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1286,9 +1284,9 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="10734216" y="1572308"/>
+              <a:off x="10734216" y="1642483"/>
               <a:ext cx="239684" cy="215559"/>
-              <a:chOff x="6932276" y="2645702"/>
+              <a:chOff x="6932276" y="2726016"/>
               <a:chExt cx="207790" cy="246688"/>
             </a:xfrm>
           </xdr:grpSpPr>
@@ -1305,7 +1303,7 @@
             </xdr:nvCxnSpPr>
             <xdr:spPr>
               <a:xfrm flipV="1">
-                <a:off x="6932447" y="2888393"/>
+                <a:off x="6932447" y="2968710"/>
                 <a:ext cx="207619" cy="313"/>
               </a:xfrm>
               <a:prstGeom prst="straightConnector1">
@@ -1346,7 +1344,7 @@
             </xdr:nvCxnSpPr>
             <xdr:spPr>
               <a:xfrm>
-                <a:off x="6932276" y="2645702"/>
+                <a:off x="6932276" y="2726016"/>
                 <a:ext cx="172" cy="246688"/>
               </a:xfrm>
               <a:prstGeom prst="line">
@@ -1388,10 +1386,10 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="13896470" y="2452973"/>
-            <a:ext cx="2028618" cy="308119"/>
-            <a:chOff x="13896470" y="2452973"/>
-            <a:chExt cx="2028618" cy="308119"/>
+            <a:off x="13896470" y="2506963"/>
+            <a:ext cx="2028618" cy="302720"/>
+            <a:chOff x="13896470" y="2506963"/>
+            <a:chExt cx="2028618" cy="302720"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
@@ -1407,7 +1405,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="14044979" y="2603714"/>
+              <a:off x="14044979" y="2652305"/>
               <a:ext cx="1880109" cy="157378"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1458,9 +1456,9 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="13896470" y="2452973"/>
+              <a:off x="13896470" y="2506963"/>
               <a:ext cx="200518" cy="123880"/>
-              <a:chOff x="5733174" y="2779131"/>
+              <a:chOff x="5733174" y="2852422"/>
               <a:chExt cx="247944" cy="168164"/>
             </a:xfrm>
           </xdr:grpSpPr>
@@ -1477,7 +1475,7 @@
             </xdr:nvCxnSpPr>
             <xdr:spPr>
               <a:xfrm flipH="1">
-                <a:off x="5980035" y="2779131"/>
+                <a:off x="5980035" y="2852422"/>
                 <a:ext cx="1083" cy="168164"/>
               </a:xfrm>
               <a:prstGeom prst="straightConnector1">
@@ -1518,7 +1516,7 @@
             </xdr:nvCxnSpPr>
             <xdr:spPr>
               <a:xfrm>
-                <a:off x="5733174" y="2784156"/>
+                <a:off x="5733174" y="2857447"/>
                 <a:ext cx="247253" cy="350"/>
               </a:xfrm>
               <a:prstGeom prst="line">
@@ -1560,10 +1558,10 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="9882280" y="1414000"/>
-            <a:ext cx="1223141" cy="189853"/>
-            <a:chOff x="9882280" y="1414000"/>
-            <a:chExt cx="1223141" cy="189853"/>
+            <a:off x="9882280" y="1444929"/>
+            <a:ext cx="1223141" cy="245307"/>
+            <a:chOff x="9882280" y="1444929"/>
+            <a:chExt cx="1223141" cy="245307"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:grpSp>
@@ -1579,10 +1577,10 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="9882280" y="1414000"/>
-              <a:ext cx="241837" cy="143750"/>
-              <a:chOff x="6956035" y="2713130"/>
-              <a:chExt cx="209656" cy="159618"/>
+              <a:off x="9882280" y="1444929"/>
+              <a:ext cx="241837" cy="199222"/>
+              <a:chOff x="6956035" y="2747456"/>
+              <a:chExt cx="209656" cy="221212"/>
             </a:xfrm>
           </xdr:grpSpPr>
           <xdr:cxnSp macro="">
@@ -1598,7 +1596,7 @@
             </xdr:nvCxnSpPr>
             <xdr:spPr>
               <a:xfrm>
-                <a:off x="6956035" y="2868938"/>
+                <a:off x="6956035" y="2964858"/>
                 <a:ext cx="209656" cy="3810"/>
               </a:xfrm>
               <a:prstGeom prst="straightConnector1">
@@ -1638,9 +1636,9 @@
               <xdr:cNvCxnSpPr/>
             </xdr:nvCxnSpPr>
             <xdr:spPr>
-              <a:xfrm>
-                <a:off x="6957682" y="2713130"/>
-                <a:ext cx="146" cy="155526"/>
+              <a:xfrm flipH="1">
+                <a:off x="6957828" y="2747456"/>
+                <a:ext cx="2413" cy="217120"/>
               </a:xfrm>
               <a:prstGeom prst="line">
                 <a:avLst/>
@@ -1680,7 +1678,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10153127" y="1505204"/>
+              <a:off x="10153127" y="1591587"/>
               <a:ext cx="952294" cy="98649"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1731,7 +1729,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10602404" y="1514839"/>
+              <a:off x="10602404" y="1601223"/>
               <a:ext cx="110882" cy="75897"/>
             </a:xfrm>
             <a:prstGeom prst="diamond">
@@ -1785,9 +1783,9 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="12735884" y="2295735"/>
+            <a:off x="12735884" y="2349725"/>
             <a:ext cx="1161205" cy="218671"/>
-            <a:chOff x="12735884" y="2295735"/>
+            <a:chOff x="12735884" y="2349725"/>
             <a:chExt cx="1161205" cy="218671"/>
           </a:xfrm>
         </xdr:grpSpPr>
@@ -1804,7 +1802,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="12951108" y="2410986"/>
+              <a:off x="12951108" y="2464976"/>
               <a:ext cx="945981" cy="103420"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1855,9 +1853,9 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="12735884" y="2295735"/>
+              <a:off x="12735884" y="2349725"/>
               <a:ext cx="176771" cy="147369"/>
-              <a:chOff x="13949677" y="2055147"/>
+              <a:chOff x="13949677" y="2103297"/>
               <a:chExt cx="180573" cy="131429"/>
             </a:xfrm>
           </xdr:grpSpPr>
@@ -1874,7 +1872,7 @@
             </xdr:nvCxnSpPr>
             <xdr:spPr>
               <a:xfrm flipV="1">
-                <a:off x="13949677" y="2185486"/>
+                <a:off x="13949677" y="2233636"/>
                 <a:ext cx="180573" cy="1090"/>
               </a:xfrm>
               <a:prstGeom prst="straightConnector1">
@@ -1915,7 +1913,7 @@
             </xdr:nvCxnSpPr>
             <xdr:spPr>
               <a:xfrm>
-                <a:off x="13952311" y="2055147"/>
+                <a:off x="13952311" y="2103297"/>
                 <a:ext cx="1679" cy="128564"/>
               </a:xfrm>
               <a:prstGeom prst="line">
@@ -1956,7 +1954,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="13386202" y="2417560"/>
+              <a:off x="13386202" y="2471549"/>
               <a:ext cx="119917" cy="81542"/>
             </a:xfrm>
             <a:prstGeom prst="diamond">
@@ -2010,10 +2008,10 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="11799913" y="2015911"/>
-            <a:ext cx="2157446" cy="289080"/>
-            <a:chOff x="11799913" y="2015911"/>
-            <a:chExt cx="2157446" cy="289080"/>
+            <a:off x="11799913" y="2086098"/>
+            <a:ext cx="2157446" cy="287397"/>
+            <a:chOff x="11799913" y="2086098"/>
+            <a:chExt cx="2157446" cy="287397"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
@@ -2029,8 +2027,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="11799913" y="2170740"/>
-              <a:ext cx="2157446" cy="134251"/>
+              <a:off x="11799913" y="2219331"/>
+              <a:ext cx="2157446" cy="154164"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2080,7 +2078,7 @@
           </xdr:nvCxnSpPr>
           <xdr:spPr>
             <a:xfrm flipH="1">
-              <a:off x="12222065" y="2015911"/>
+              <a:off x="12222065" y="2086098"/>
               <a:ext cx="2895" cy="121557"/>
             </a:xfrm>
             <a:prstGeom prst="straightConnector1">
@@ -2121,7 +2119,7 @@
           </xdr:nvCxnSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="12079534" y="2018832"/>
+              <a:off x="12079534" y="2089019"/>
               <a:ext cx="145425" cy="291"/>
             </a:xfrm>
             <a:prstGeom prst="line">
@@ -2162,10 +2160,10 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="11127098" y="1857984"/>
-            <a:ext cx="975407" cy="207061"/>
-            <a:chOff x="11127098" y="1857984"/>
-            <a:chExt cx="975407" cy="207061"/>
+            <a:off x="11127098" y="1922724"/>
+            <a:ext cx="975407" cy="212507"/>
+            <a:chOff x="11127098" y="1922724"/>
+            <a:chExt cx="975407" cy="212507"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
@@ -2181,7 +2179,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="11289001" y="1961307"/>
+              <a:off x="11289001" y="2031493"/>
               <a:ext cx="813504" cy="103738"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2232,10 +2230,10 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="11127098" y="1857984"/>
-              <a:ext cx="161904" cy="155180"/>
-              <a:chOff x="6977263" y="2756190"/>
-              <a:chExt cx="140694" cy="172640"/>
+              <a:off x="11127098" y="1922724"/>
+              <a:ext cx="161904" cy="160585"/>
+              <a:chOff x="6977263" y="2828262"/>
+              <a:chExt cx="140694" cy="178656"/>
             </a:xfrm>
           </xdr:grpSpPr>
           <xdr:cxnSp macro="">
@@ -2253,7 +2251,7 @@
             </xdr:nvCxnSpPr>
             <xdr:spPr>
               <a:xfrm>
-                <a:off x="6977263" y="2928299"/>
+                <a:off x="6977263" y="3006387"/>
                 <a:ext cx="140694" cy="531"/>
               </a:xfrm>
               <a:prstGeom prst="straightConnector1">
@@ -2294,7 +2292,7 @@
             </xdr:nvCxnSpPr>
             <xdr:spPr>
               <a:xfrm>
-                <a:off x="6979851" y="2756190"/>
+                <a:off x="6979851" y="2828262"/>
                 <a:ext cx="1081" cy="172108"/>
               </a:xfrm>
               <a:prstGeom prst="line">
@@ -2335,7 +2333,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="11631077" y="1977366"/>
+              <a:off x="11631077" y="2047553"/>
               <a:ext cx="99841" cy="67126"/>
             </a:xfrm>
             <a:prstGeom prst="diamond">
@@ -3063,8 +3061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C326E24E-2340-7440-93FB-5CAF133542E1}">
   <dimension ref="A1:AU19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3125,159 +3123,159 @@
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
-      <c r="AA2" s="35"/>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="35"/>
-      <c r="AH2" s="35"/>
-      <c r="AI2" s="35"/>
-      <c r="AJ2" s="35"/>
-      <c r="AK2" s="35"/>
-      <c r="AL2" s="35"/>
-      <c r="AM2" s="35"/>
-      <c r="AN2" s="35"/>
-      <c r="AO2" s="35"/>
-      <c r="AP2" s="35"/>
-      <c r="AQ2" s="35"/>
-      <c r="AR2" s="35"/>
-      <c r="AS2" s="35"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
+      <c r="AO2" s="38"/>
+      <c r="AP2" s="38"/>
+      <c r="AQ2" s="38"/>
+      <c r="AR2" s="38"/>
+      <c r="AS2" s="38"/>
       <c r="AT2" s="21"/>
       <c r="AU2" s="10"/>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" s="20"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33">
+      <c r="B3" s="33"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="29">
         <v>1</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33">
+      <c r="G3" s="29"/>
+      <c r="H3" s="29">
         <v>2</v>
       </c>
-      <c r="I3" s="33">
+      <c r="I3" s="29">
         <v>2</v>
       </c>
-      <c r="J3" s="33">
+      <c r="J3" s="29">
         <v>3</v>
       </c>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33">
+      <c r="K3" s="29"/>
+      <c r="L3" s="29">
         <v>4</v>
       </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33">
+      <c r="M3" s="29"/>
+      <c r="N3" s="29">
         <v>5</v>
       </c>
-      <c r="O3" s="33">
+      <c r="O3" s="29">
         <v>4</v>
       </c>
-      <c r="P3" s="33">
+      <c r="P3" s="29">
         <v>6</v>
       </c>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33">
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29">
         <v>7</v>
       </c>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33">
+      <c r="S3" s="29"/>
+      <c r="T3" s="29">
         <v>8</v>
       </c>
-      <c r="U3" s="33">
+      <c r="U3" s="29">
         <v>6</v>
       </c>
-      <c r="V3" s="33">
+      <c r="V3" s="29">
         <v>9</v>
       </c>
-      <c r="W3" s="33"/>
-      <c r="X3" s="33">
+      <c r="W3" s="29"/>
+      <c r="X3" s="29">
         <v>10</v>
       </c>
-      <c r="Y3" s="33"/>
-      <c r="Z3" s="33">
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="29">
         <v>11</v>
       </c>
-      <c r="AA3" s="33">
+      <c r="AA3" s="29">
         <v>8</v>
       </c>
-      <c r="AB3" s="33">
+      <c r="AB3" s="29">
         <v>12</v>
       </c>
-      <c r="AC3" s="33"/>
-      <c r="AD3" s="33">
+      <c r="AC3" s="29"/>
+      <c r="AD3" s="29">
         <v>13</v>
       </c>
-      <c r="AE3" s="33"/>
-      <c r="AF3" s="33">
+      <c r="AE3" s="29"/>
+      <c r="AF3" s="29">
         <v>14</v>
       </c>
-      <c r="AG3" s="33">
+      <c r="AG3" s="29">
         <v>10</v>
       </c>
-      <c r="AH3" s="33">
+      <c r="AH3" s="29">
         <v>15</v>
       </c>
-      <c r="AI3" s="33"/>
-      <c r="AJ3" s="33">
+      <c r="AI3" s="29"/>
+      <c r="AJ3" s="29">
         <v>16</v>
       </c>
-      <c r="AK3" s="33"/>
-      <c r="AL3" s="33">
+      <c r="AK3" s="29"/>
+      <c r="AL3" s="29">
         <v>17</v>
       </c>
-      <c r="AM3" s="33"/>
-      <c r="AN3" s="33">
+      <c r="AM3" s="29"/>
+      <c r="AN3" s="29">
         <v>18</v>
       </c>
-      <c r="AO3" s="33"/>
-      <c r="AP3" s="33">
+      <c r="AO3" s="29"/>
+      <c r="AP3" s="29">
         <v>19</v>
       </c>
-      <c r="AQ3" s="33"/>
-      <c r="AR3" s="33">
+      <c r="AQ3" s="29"/>
+      <c r="AR3" s="29">
         <v>20</v>
       </c>
-      <c r="AS3" s="33"/>
+      <c r="AS3" s="29"/>
       <c r="AT3" s="21"/>
       <c r="AU3" s="10"/>
     </row>
@@ -3295,46 +3293,46 @@
       <c r="E4" s="5">
         <v>15</v>
       </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="34"/>
-      <c r="W4" s="34"/>
-      <c r="X4" s="34"/>
-      <c r="Y4" s="34"/>
-      <c r="Z4" s="34"/>
-      <c r="AA4" s="34"/>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
-      <c r="AG4" s="34"/>
-      <c r="AH4" s="34"/>
-      <c r="AI4" s="34"/>
-      <c r="AJ4" s="34"/>
-      <c r="AK4" s="34"/>
-      <c r="AL4" s="34"/>
-      <c r="AM4" s="34"/>
-      <c r="AN4" s="34"/>
-      <c r="AO4" s="34"/>
-      <c r="AP4" s="34"/>
-      <c r="AQ4" s="34"/>
-      <c r="AR4" s="34"/>
-      <c r="AS4" s="34"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AD4" s="25"/>
+      <c r="AE4" s="25"/>
+      <c r="AF4" s="25"/>
+      <c r="AG4" s="25"/>
+      <c r="AH4" s="25"/>
+      <c r="AI4" s="25"/>
+      <c r="AJ4" s="25"/>
+      <c r="AK4" s="25"/>
+      <c r="AL4" s="25"/>
+      <c r="AM4" s="25"/>
+      <c r="AN4" s="25"/>
+      <c r="AO4" s="25"/>
+      <c r="AP4" s="25"/>
+      <c r="AQ4" s="25"/>
+      <c r="AR4" s="25"/>
+      <c r="AS4" s="25"/>
       <c r="AT4" s="21"/>
       <c r="AU4" s="10"/>
     </row>
@@ -3352,46 +3350,46 @@
       <c r="E5" s="3">
         <v>4</v>
       </c>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="34"/>
-      <c r="W5" s="34"/>
-      <c r="X5" s="34"/>
-      <c r="Y5" s="34"/>
-      <c r="Z5" s="34"/>
-      <c r="AA5" s="34"/>
-      <c r="AB5" s="34"/>
-      <c r="AC5" s="34"/>
-      <c r="AD5" s="34"/>
-      <c r="AE5" s="34"/>
-      <c r="AF5" s="34"/>
-      <c r="AG5" s="34"/>
-      <c r="AH5" s="34"/>
-      <c r="AI5" s="34"/>
-      <c r="AJ5" s="34"/>
-      <c r="AK5" s="34"/>
-      <c r="AL5" s="34"/>
-      <c r="AM5" s="34"/>
-      <c r="AN5" s="34"/>
-      <c r="AO5" s="34"/>
-      <c r="AP5" s="34"/>
-      <c r="AQ5" s="34"/>
-      <c r="AR5" s="34"/>
-      <c r="AS5" s="34"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="25"/>
+      <c r="AB5" s="25"/>
+      <c r="AC5" s="25"/>
+      <c r="AD5" s="25"/>
+      <c r="AE5" s="25"/>
+      <c r="AF5" s="25"/>
+      <c r="AG5" s="25"/>
+      <c r="AH5" s="25"/>
+      <c r="AI5" s="25"/>
+      <c r="AJ5" s="25"/>
+      <c r="AK5" s="25"/>
+      <c r="AL5" s="25"/>
+      <c r="AM5" s="25"/>
+      <c r="AN5" s="25"/>
+      <c r="AO5" s="25"/>
+      <c r="AP5" s="25"/>
+      <c r="AQ5" s="25"/>
+      <c r="AR5" s="25"/>
+      <c r="AS5" s="25"/>
       <c r="AT5" s="21"/>
       <c r="AU5" s="10"/>
     </row>
@@ -3409,53 +3407,53 @@
       <c r="E6" s="3">
         <v>3</v>
       </c>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="34"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34"/>
-      <c r="U6" s="34"/>
-      <c r="V6" s="34"/>
-      <c r="W6" s="34"/>
-      <c r="X6" s="34"/>
-      <c r="Y6" s="34"/>
-      <c r="Z6" s="34"/>
-      <c r="AA6" s="34"/>
-      <c r="AB6" s="34"/>
-      <c r="AC6" s="34"/>
-      <c r="AD6" s="34"/>
-      <c r="AE6" s="34"/>
-      <c r="AF6" s="34"/>
-      <c r="AG6" s="34"/>
-      <c r="AH6" s="34"/>
-      <c r="AI6" s="34"/>
-      <c r="AJ6" s="34"/>
-      <c r="AK6" s="34"/>
-      <c r="AL6" s="34"/>
-      <c r="AM6" s="34"/>
-      <c r="AN6" s="34"/>
-      <c r="AO6" s="34"/>
-      <c r="AP6" s="34"/>
-      <c r="AQ6" s="34"/>
-      <c r="AR6" s="34"/>
-      <c r="AS6" s="34"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="25"/>
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="25"/>
+      <c r="AD6" s="25"/>
+      <c r="AE6" s="25"/>
+      <c r="AF6" s="25"/>
+      <c r="AG6" s="25"/>
+      <c r="AH6" s="25"/>
+      <c r="AI6" s="25"/>
+      <c r="AJ6" s="25"/>
+      <c r="AK6" s="25"/>
+      <c r="AL6" s="25"/>
+      <c r="AM6" s="25"/>
+      <c r="AN6" s="25"/>
+      <c r="AO6" s="25"/>
+      <c r="AP6" s="25"/>
+      <c r="AQ6" s="25"/>
+      <c r="AR6" s="25"/>
+      <c r="AS6" s="25"/>
       <c r="AT6" s="21"/>
       <c r="AU6" s="10"/>
     </row>
-    <row r="7" spans="1:47" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:47" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="20"/>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7" s="4">
         <v>44997</v>
@@ -3569,7 +3567,7 @@
     <row r="9" spans="1:47" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="20"/>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4">
         <v>45021</v>
@@ -3637,53 +3635,53 @@
       <c r="E10" s="3">
         <v>4</v>
       </c>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
-      <c r="T10" s="34"/>
-      <c r="U10" s="34"/>
-      <c r="V10" s="34"/>
-      <c r="W10" s="34"/>
-      <c r="X10" s="34"/>
-      <c r="Y10" s="34"/>
-      <c r="Z10" s="34"/>
-      <c r="AA10" s="34"/>
-      <c r="AB10" s="34"/>
-      <c r="AC10" s="34"/>
-      <c r="AD10" s="34"/>
-      <c r="AE10" s="34"/>
-      <c r="AF10" s="34"/>
-      <c r="AG10" s="34"/>
-      <c r="AH10" s="34"/>
-      <c r="AI10" s="34"/>
-      <c r="AJ10" s="34"/>
-      <c r="AK10" s="34"/>
-      <c r="AL10" s="34"/>
-      <c r="AM10" s="34"/>
-      <c r="AN10" s="34"/>
-      <c r="AO10" s="34"/>
-      <c r="AP10" s="34"/>
-      <c r="AQ10" s="34"/>
-      <c r="AR10" s="34"/>
-      <c r="AS10" s="34"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+      <c r="AA10" s="25"/>
+      <c r="AB10" s="25"/>
+      <c r="AC10" s="25"/>
+      <c r="AD10" s="25"/>
+      <c r="AE10" s="25"/>
+      <c r="AF10" s="25"/>
+      <c r="AG10" s="25"/>
+      <c r="AH10" s="25"/>
+      <c r="AI10" s="25"/>
+      <c r="AJ10" s="25"/>
+      <c r="AK10" s="25"/>
+      <c r="AL10" s="25"/>
+      <c r="AM10" s="25"/>
+      <c r="AN10" s="25"/>
+      <c r="AO10" s="25"/>
+      <c r="AP10" s="25"/>
+      <c r="AQ10" s="25"/>
+      <c r="AR10" s="25"/>
+      <c r="AS10" s="25"/>
       <c r="AT10" s="21"/>
       <c r="AU10" s="10"/>
     </row>
     <row r="11" spans="1:47" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="20"/>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="9">
         <v>45032</v>
@@ -3700,10 +3698,10 @@
       <c r="I11" s="23"/>
       <c r="J11" s="22"/>
       <c r="K11" s="23"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="26"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="31"/>
       <c r="P11" s="22"/>
       <c r="Q11" s="23"/>
       <c r="R11" s="22"/>
@@ -3797,7 +3795,7 @@
     <row r="13" spans="1:47" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="20"/>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="4">
         <v>45060</v>
@@ -4154,56 +4152,56 @@
       <c r="E18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="36">
+      <c r="F18" s="26">
         <v>2</v>
       </c>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="36">
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="26">
         <v>3</v>
       </c>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="37"/>
-      <c r="T18" s="38"/>
-      <c r="U18" s="36">
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="26">
         <v>4</v>
       </c>
-      <c r="V18" s="37"/>
-      <c r="W18" s="37"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="37"/>
-      <c r="Z18" s="37"/>
-      <c r="AA18" s="37"/>
-      <c r="AB18" s="37"/>
-      <c r="AC18" s="37"/>
-      <c r="AD18" s="38"/>
-      <c r="AE18" s="36">
+      <c r="V18" s="27"/>
+      <c r="W18" s="27"/>
+      <c r="X18" s="27"/>
+      <c r="Y18" s="27"/>
+      <c r="Z18" s="27"/>
+      <c r="AA18" s="27"/>
+      <c r="AB18" s="27"/>
+      <c r="AC18" s="27"/>
+      <c r="AD18" s="28"/>
+      <c r="AE18" s="26">
         <v>5</v>
       </c>
-      <c r="AF18" s="37"/>
-      <c r="AG18" s="37"/>
-      <c r="AH18" s="37"/>
-      <c r="AI18" s="37"/>
-      <c r="AJ18" s="37"/>
-      <c r="AK18" s="37"/>
-      <c r="AL18" s="38"/>
-      <c r="AM18" s="36">
+      <c r="AF18" s="27"/>
+      <c r="AG18" s="27"/>
+      <c r="AH18" s="27"/>
+      <c r="AI18" s="27"/>
+      <c r="AJ18" s="27"/>
+      <c r="AK18" s="27"/>
+      <c r="AL18" s="28"/>
+      <c r="AM18" s="26">
         <v>6</v>
       </c>
-      <c r="AN18" s="37"/>
-      <c r="AO18" s="37"/>
-      <c r="AP18" s="37"/>
-      <c r="AQ18" s="37"/>
-      <c r="AR18" s="37"/>
-      <c r="AS18" s="38"/>
+      <c r="AN18" s="27"/>
+      <c r="AO18" s="27"/>
+      <c r="AP18" s="27"/>
+      <c r="AQ18" s="27"/>
+      <c r="AR18" s="27"/>
+      <c r="AS18" s="28"/>
       <c r="AT18" s="20"/>
     </row>
     <row r="19" spans="1:46" x14ac:dyDescent="0.2">
@@ -4256,44 +4254,56 @@
     </row>
   </sheetData>
   <mergeCells count="112">
-    <mergeCell ref="AN6:AO6"/>
-    <mergeCell ref="AP6:AQ6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="AR6:AS6"/>
-    <mergeCell ref="AF6:AG6"/>
-    <mergeCell ref="AH6:AI6"/>
-    <mergeCell ref="F18:L18"/>
-    <mergeCell ref="M18:T18"/>
-    <mergeCell ref="U18:AD18"/>
-    <mergeCell ref="AE18:AL18"/>
-    <mergeCell ref="AM18:AS18"/>
-    <mergeCell ref="AH5:AI5"/>
-    <mergeCell ref="AJ5:AK5"/>
-    <mergeCell ref="AL5:AM5"/>
-    <mergeCell ref="AN5:AO5"/>
-    <mergeCell ref="AP5:AQ5"/>
-    <mergeCell ref="AR5:AS5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="AJ6:AK6"/>
-    <mergeCell ref="AL6:AM6"/>
-    <mergeCell ref="T10:U10"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="X10:Y10"/>
-    <mergeCell ref="Z10:AA10"/>
-    <mergeCell ref="AB10:AC10"/>
-    <mergeCell ref="AD10:AE10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="AN10:AO10"/>
+    <mergeCell ref="AP10:AQ10"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AH4:AI4"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="F2:AS2"/>
+    <mergeCell ref="AR10:AS10"/>
+    <mergeCell ref="AF10:AG10"/>
+    <mergeCell ref="AH10:AI10"/>
+    <mergeCell ref="AJ10:AK10"/>
+    <mergeCell ref="AL10:AM10"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AR3:AS3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AP4:AQ4"/>
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="R10:S10"/>
     <mergeCell ref="AJ4:AK4"/>
@@ -4318,56 +4328,44 @@
     <mergeCell ref="V6:W6"/>
     <mergeCell ref="X6:Y6"/>
     <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="AR3:AS3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AP4:AQ4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AH4:AI4"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="F2:AS2"/>
-    <mergeCell ref="AR10:AS10"/>
-    <mergeCell ref="AF10:AG10"/>
-    <mergeCell ref="AH10:AI10"/>
-    <mergeCell ref="AJ10:AK10"/>
-    <mergeCell ref="AL10:AM10"/>
-    <mergeCell ref="AN10:AO10"/>
-    <mergeCell ref="AP10:AQ10"/>
+    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="AL5:AM5"/>
+    <mergeCell ref="AN5:AO5"/>
+    <mergeCell ref="AP5:AQ5"/>
+    <mergeCell ref="AR5:AS5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="AN6:AO6"/>
+    <mergeCell ref="AP6:AQ6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="AR6:AS6"/>
+    <mergeCell ref="AF6:AG6"/>
+    <mergeCell ref="AH6:AI6"/>
+    <mergeCell ref="F18:L18"/>
+    <mergeCell ref="M18:T18"/>
+    <mergeCell ref="U18:AD18"/>
+    <mergeCell ref="AE18:AL18"/>
+    <mergeCell ref="AM18:AS18"/>
+    <mergeCell ref="AJ6:AK6"/>
+    <mergeCell ref="AL6:AM6"/>
+    <mergeCell ref="T10:U10"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="X10:Y10"/>
+    <mergeCell ref="Z10:AA10"/>
+    <mergeCell ref="AB10:AC10"/>
+    <mergeCell ref="AD10:AE10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:O10"/>
   </mergeCells>
   <conditionalFormatting sqref="AN5 AP5 AR5 AN13 AP13 AR13 AN9:AN10 AP9:AP10 AR9:AR10 F5:F16 H5:H16 J5:J16 L5:L16 N5:N16 P5:P16 R5:R16 T5:T16 V5:V16 X5:X16 Z5:Z16 AB5:AB16 AD5:AD16 AF5:AF16 AH5:AH16 AJ5:AJ16 AL5:AL16 AN16 AP16 AR16">
     <cfRule type="dataBar" priority="58">

</xml_diff>

<commit_message>
Codigo do servidor, proposal, foto de ligaçao de rele com sensor de tensao
UPDATES
</commit_message>
<xml_diff>
--- a/Diagrama Gant.xlsx
+++ b/Diagrama Gant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelabreu/Desktop/Smart metering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB1C25A-AF68-B54A-9039-F3205EB6B98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82A64D5-B378-4B4F-865B-E0E1090C27F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{AC57B2E7-C3B7-485D-9028-5182123DD5F2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Trabalho de pesquisa</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Implementação do transformador 230V AC para 5V DC e determinação e amostragem no servidor online do preço associado ao consumo de energia elétrica</t>
+  </si>
+  <si>
+    <t>Testagem do hardware necessário para o desenvolver do projeto, nomeadamente sensores de tensão, corrente, temperatura e os relés</t>
   </si>
 </sst>
 </file>
@@ -307,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -367,6 +370,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -386,19 +398,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -445,8 +454,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6293443" y="619260"/>
-          <a:ext cx="2124376" cy="282440"/>
+          <a:off x="6310376" y="606560"/>
+          <a:ext cx="2183643" cy="290907"/>
           <a:chOff x="5470236" y="522812"/>
           <a:chExt cx="2041379" cy="207700"/>
         </a:xfrm>
@@ -700,8 +709,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8955099" y="1105577"/>
-          <a:ext cx="170758" cy="296865"/>
+          <a:off x="9048232" y="1101344"/>
+          <a:ext cx="179225" cy="296865"/>
           <a:chOff x="7467947" y="2668507"/>
           <a:chExt cx="420214" cy="124669"/>
         </a:xfrm>
@@ -860,13 +869,13 @@
     <xdr:from>
       <xdr:col>39</xdr:col>
       <xdr:colOff>49869</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>190047</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>245532</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>575733</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -926,13 +935,13 @@
     <xdr:from>
       <xdr:col>38</xdr:col>
       <xdr:colOff>124322</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>310041</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>39</xdr:col>
       <xdr:colOff>31821</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>403234</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -948,8 +957,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="15542122" y="3954941"/>
-          <a:ext cx="186899" cy="499593"/>
+          <a:off x="15838455" y="4763508"/>
+          <a:ext cx="195366" cy="499593"/>
           <a:chOff x="15554535" y="2384381"/>
           <a:chExt cx="187396" cy="184858"/>
         </a:xfrm>
@@ -1219,13 +1228,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>97337</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>164373</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>245865</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>472813</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1241,8 +1250,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10765337" y="2183673"/>
-          <a:ext cx="986728" cy="511640"/>
+          <a:off x="10917737" y="2992240"/>
+          <a:ext cx="1012128" cy="511640"/>
           <a:chOff x="10734216" y="1642483"/>
           <a:chExt cx="984762" cy="295857"/>
         </a:xfrm>
@@ -1406,13 +1415,13 @@
     <xdr:from>
       <xdr:col>33</xdr:col>
       <xdr:colOff>64031</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>107289</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>39</xdr:col>
       <xdr:colOff>272154</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>342939</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1472,13 +1481,13 @@
     <xdr:from>
       <xdr:col>32</xdr:col>
       <xdr:colOff>194295</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>88126</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
       <xdr:colOff>116074</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>100104</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1494,8 +1503,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13935695" y="3529826"/>
-          <a:ext cx="201179" cy="215178"/>
+          <a:off x="14181228" y="4338393"/>
+          <a:ext cx="209646" cy="215178"/>
           <a:chOff x="5733174" y="2852422"/>
           <a:chExt cx="247944" cy="168164"/>
         </a:xfrm>
@@ -1587,14 +1596,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>66898</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>497114</xdr:rowOff>
+      <xdr:colOff>65686</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>29883</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:colOff>29876</xdr:colOff>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>106033</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1610,10 +1619,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9896698" y="1703614"/>
-          <a:ext cx="242385" cy="421719"/>
-          <a:chOff x="6956035" y="2747456"/>
-          <a:chExt cx="209656" cy="221212"/>
+          <a:off x="10022486" y="2386542"/>
+          <a:ext cx="252057" cy="547358"/>
+          <a:chOff x="6956035" y="1802876"/>
+          <a:chExt cx="209656" cy="1165792"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
@@ -1670,8 +1679,8 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm flipH="1">
-            <a:off x="6957828" y="2747456"/>
-            <a:ext cx="2413" cy="217120"/>
+            <a:off x="6957827" y="1802876"/>
+            <a:ext cx="1792" cy="1161701"/>
           </a:xfrm>
           <a:prstGeom prst="line">
             <a:avLst/>
@@ -1704,13 +1713,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>58959</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>29028</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>175211</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>170950</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1770,13 +1779,13 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>199570</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>42929</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>25301</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>148771</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1838,13 +1847,13 @@
     <xdr:from>
       <xdr:col>29</xdr:col>
       <xdr:colOff>87506</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>30149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>197494</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>165184</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1904,13 +1913,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>183722</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>251480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>82927</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>94940</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1926,8 +1935,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12807522" y="3286780"/>
-          <a:ext cx="178605" cy="249860"/>
+          <a:off x="13019189" y="4095347"/>
+          <a:ext cx="187071" cy="249860"/>
           <a:chOff x="13948463" y="2105245"/>
           <a:chExt cx="181787" cy="129481"/>
         </a:xfrm>
@@ -2020,13 +2029,13 @@
     <xdr:from>
       <xdr:col>30</xdr:col>
       <xdr:colOff>232708</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>48988</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>48990</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>138777</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2088,13 +2097,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>44843</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>85442</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>251312</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>344298</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2110,8 +2119,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11830443" y="2917542"/>
-          <a:ext cx="2162269" cy="462056"/>
+          <a:off x="12016710" y="3726109"/>
+          <a:ext cx="2221535" cy="462056"/>
           <a:chOff x="11799913" y="2105633"/>
           <a:chExt cx="2157446" cy="267862"/>
         </a:xfrm>
@@ -2255,13 +2264,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>87578</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>31910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>65543</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>156108</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2321,13 +2330,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>210627</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>434842</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>87602</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>94001</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2343,8 +2352,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11158027" y="2657342"/>
-          <a:ext cx="156375" cy="268759"/>
+          <a:off x="11318894" y="3465909"/>
+          <a:ext cx="164841" cy="268759"/>
           <a:chOff x="6979698" y="2828262"/>
           <a:chExt cx="135490" cy="173630"/>
         </a:xfrm>
@@ -2439,13 +2448,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>175501</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>51055</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>257922</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>127638</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2507,13 +2516,13 @@
     <xdr:from>
       <xdr:col>41</xdr:col>
       <xdr:colOff>61214</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>39178</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>44</xdr:col>
       <xdr:colOff>223861</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>157512</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2573,13 +2582,13 @@
     <xdr:from>
       <xdr:col>40</xdr:col>
       <xdr:colOff>137905</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>98676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
       <xdr:colOff>52906</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>100497</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2629,13 +2638,13 @@
     <xdr:from>
       <xdr:col>42</xdr:col>
       <xdr:colOff>84884</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>39177</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>44</xdr:col>
       <xdr:colOff>234252</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>147063</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2695,13 +2704,13 @@
     <xdr:from>
       <xdr:col>41</xdr:col>
       <xdr:colOff>191628</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>93120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>84884</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>93935</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2753,13 +2762,13 @@
     <xdr:from>
       <xdr:col>40</xdr:col>
       <xdr:colOff>134932</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>491120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>138765</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>102568</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2808,13 +2817,13 @@
     <xdr:from>
       <xdr:col>42</xdr:col>
       <xdr:colOff>246722</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>52238</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
       <xdr:colOff>42443</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>129701</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2944,13 +2953,13 @@
     <xdr:from>
       <xdr:col>41</xdr:col>
       <xdr:colOff>191628</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>131509</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
       <xdr:colOff>193473</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>97158</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2993,6 +3002,128 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>81935</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>450645</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>87056</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>128024</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conexão Reta Unidirecional 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CF192B9-8E6A-9147-86A1-76475A0E87D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9663266" y="1659193"/>
+          <a:ext cx="5121" cy="491613"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>61452</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>168992</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>179235</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>469903</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Retângulo 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{733203AF-F4F7-3F4F-B980-76644F72E2EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9642783" y="2191774"/>
+          <a:ext cx="399436" cy="300911"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-PT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3295,10 +3426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C326E24E-2340-7440-93FB-5CAF133542E1}">
-  <dimension ref="A1:AU19"/>
+  <dimension ref="A1:AU20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3359,159 +3490,159 @@
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="32"/>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="34"/>
+      <c r="AA2" s="34"/>
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="34"/>
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="34"/>
+      <c r="AH2" s="34"/>
+      <c r="AI2" s="34"/>
+      <c r="AJ2" s="34"/>
+      <c r="AK2" s="34"/>
+      <c r="AL2" s="34"/>
+      <c r="AM2" s="34"/>
+      <c r="AN2" s="34"/>
+      <c r="AO2" s="34"/>
+      <c r="AP2" s="34"/>
+      <c r="AQ2" s="34"/>
+      <c r="AR2" s="34"/>
+      <c r="AS2" s="34"/>
       <c r="AT2" s="21"/>
       <c r="AU2" s="10"/>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" s="20"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31">
+      <c r="B3" s="29"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="27">
         <v>1</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31">
+      <c r="G3" s="27"/>
+      <c r="H3" s="27">
         <v>2</v>
       </c>
-      <c r="I3" s="31">
+      <c r="I3" s="27">
         <v>2</v>
       </c>
-      <c r="J3" s="31">
+      <c r="J3" s="27">
         <v>3</v>
       </c>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31">
+      <c r="K3" s="27"/>
+      <c r="L3" s="27">
         <v>4</v>
       </c>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31">
+      <c r="M3" s="27"/>
+      <c r="N3" s="27">
         <v>5</v>
       </c>
-      <c r="O3" s="31">
+      <c r="O3" s="27">
         <v>4</v>
       </c>
-      <c r="P3" s="31">
+      <c r="P3" s="27">
         <v>6</v>
       </c>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31">
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27">
         <v>7</v>
       </c>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31">
+      <c r="S3" s="27"/>
+      <c r="T3" s="27">
         <v>8</v>
       </c>
-      <c r="U3" s="31">
+      <c r="U3" s="27">
         <v>6</v>
       </c>
-      <c r="V3" s="31">
+      <c r="V3" s="27">
         <v>9</v>
       </c>
-      <c r="W3" s="31"/>
-      <c r="X3" s="31">
+      <c r="W3" s="27"/>
+      <c r="X3" s="27">
         <v>10</v>
       </c>
-      <c r="Y3" s="31"/>
-      <c r="Z3" s="31">
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27">
         <v>11</v>
       </c>
-      <c r="AA3" s="31">
+      <c r="AA3" s="27">
         <v>8</v>
       </c>
-      <c r="AB3" s="31">
+      <c r="AB3" s="27">
         <v>12</v>
       </c>
-      <c r="AC3" s="31"/>
-      <c r="AD3" s="31">
+      <c r="AC3" s="27"/>
+      <c r="AD3" s="27">
         <v>13</v>
       </c>
-      <c r="AE3" s="31"/>
-      <c r="AF3" s="31">
+      <c r="AE3" s="27"/>
+      <c r="AF3" s="27">
         <v>14</v>
       </c>
-      <c r="AG3" s="31">
+      <c r="AG3" s="27">
         <v>10</v>
       </c>
-      <c r="AH3" s="31">
+      <c r="AH3" s="27">
         <v>15</v>
       </c>
-      <c r="AI3" s="31"/>
-      <c r="AJ3" s="31">
+      <c r="AI3" s="27"/>
+      <c r="AJ3" s="27">
         <v>16</v>
       </c>
-      <c r="AK3" s="31"/>
-      <c r="AL3" s="31">
+      <c r="AK3" s="27"/>
+      <c r="AL3" s="27">
         <v>17</v>
       </c>
-      <c r="AM3" s="31"/>
-      <c r="AN3" s="31">
+      <c r="AM3" s="27"/>
+      <c r="AN3" s="27">
         <v>18</v>
       </c>
-      <c r="AO3" s="31"/>
-      <c r="AP3" s="31">
+      <c r="AO3" s="27"/>
+      <c r="AP3" s="27">
         <v>19</v>
       </c>
-      <c r="AQ3" s="31"/>
-      <c r="AR3" s="31">
+      <c r="AQ3" s="27"/>
+      <c r="AR3" s="27">
         <v>20</v>
       </c>
-      <c r="AS3" s="31"/>
+      <c r="AS3" s="27"/>
       <c r="AT3" s="21"/>
       <c r="AU3" s="10"/>
     </row>
@@ -3529,46 +3660,46 @@
       <c r="E4" s="5">
         <v>15</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="24"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="24"/>
-      <c r="AD4" s="23"/>
-      <c r="AE4" s="24"/>
-      <c r="AF4" s="23"/>
-      <c r="AG4" s="24"/>
-      <c r="AH4" s="23"/>
-      <c r="AI4" s="24"/>
-      <c r="AJ4" s="23"/>
-      <c r="AK4" s="24"/>
-      <c r="AL4" s="23"/>
-      <c r="AM4" s="24"/>
-      <c r="AN4" s="23"/>
-      <c r="AO4" s="24"/>
-      <c r="AP4" s="23"/>
-      <c r="AQ4" s="24"/>
-      <c r="AR4" s="23"/>
-      <c r="AS4" s="24"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="26"/>
+      <c r="AD4" s="25"/>
+      <c r="AE4" s="26"/>
+      <c r="AF4" s="25"/>
+      <c r="AG4" s="26"/>
+      <c r="AH4" s="25"/>
+      <c r="AI4" s="26"/>
+      <c r="AJ4" s="25"/>
+      <c r="AK4" s="26"/>
+      <c r="AL4" s="25"/>
+      <c r="AM4" s="26"/>
+      <c r="AN4" s="25"/>
+      <c r="AO4" s="26"/>
+      <c r="AP4" s="25"/>
+      <c r="AQ4" s="26"/>
+      <c r="AR4" s="25"/>
+      <c r="AS4" s="26"/>
       <c r="AT4" s="21"/>
       <c r="AU4" s="10"/>
     </row>
@@ -3586,46 +3717,46 @@
       <c r="E5" s="3">
         <v>4</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="24"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="24"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="24"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="24"/>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="24"/>
-      <c r="AD5" s="23"/>
-      <c r="AE5" s="24"/>
-      <c r="AF5" s="23"/>
-      <c r="AG5" s="24"/>
-      <c r="AH5" s="23"/>
-      <c r="AI5" s="24"/>
-      <c r="AJ5" s="23"/>
-      <c r="AK5" s="24"/>
-      <c r="AL5" s="23"/>
-      <c r="AM5" s="24"/>
-      <c r="AN5" s="23"/>
-      <c r="AO5" s="24"/>
-      <c r="AP5" s="23"/>
-      <c r="AQ5" s="24"/>
-      <c r="AR5" s="23"/>
-      <c r="AS5" s="24"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="25"/>
+      <c r="AC5" s="26"/>
+      <c r="AD5" s="25"/>
+      <c r="AE5" s="26"/>
+      <c r="AF5" s="25"/>
+      <c r="AG5" s="26"/>
+      <c r="AH5" s="25"/>
+      <c r="AI5" s="26"/>
+      <c r="AJ5" s="25"/>
+      <c r="AK5" s="26"/>
+      <c r="AL5" s="25"/>
+      <c r="AM5" s="26"/>
+      <c r="AN5" s="25"/>
+      <c r="AO5" s="26"/>
+      <c r="AP5" s="25"/>
+      <c r="AQ5" s="26"/>
+      <c r="AR5" s="25"/>
+      <c r="AS5" s="26"/>
       <c r="AT5" s="21"/>
       <c r="AU5" s="10"/>
     </row>
@@ -3643,46 +3774,46 @@
       <c r="E6" s="3">
         <v>3</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="24"/>
-      <c r="AD6" s="23"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="23"/>
-      <c r="AG6" s="24"/>
-      <c r="AH6" s="23"/>
-      <c r="AI6" s="24"/>
-      <c r="AJ6" s="23"/>
-      <c r="AK6" s="24"/>
-      <c r="AL6" s="23"/>
-      <c r="AM6" s="24"/>
-      <c r="AN6" s="23"/>
-      <c r="AO6" s="24"/>
-      <c r="AP6" s="23"/>
-      <c r="AQ6" s="24"/>
-      <c r="AR6" s="23"/>
-      <c r="AS6" s="24"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="25"/>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="25"/>
+      <c r="AG6" s="26"/>
+      <c r="AH6" s="25"/>
+      <c r="AI6" s="26"/>
+      <c r="AJ6" s="25"/>
+      <c r="AK6" s="26"/>
+      <c r="AL6" s="25"/>
+      <c r="AM6" s="26"/>
+      <c r="AN6" s="25"/>
+      <c r="AO6" s="26"/>
+      <c r="AP6" s="25"/>
+      <c r="AQ6" s="26"/>
+      <c r="AR6" s="25"/>
+      <c r="AS6" s="26"/>
       <c r="AT6" s="21"/>
       <c r="AU6" s="10"/>
     </row>
@@ -3700,176 +3831,176 @@
       <c r="E7" s="3">
         <v>22</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="24"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="24"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="24"/>
-      <c r="X7" s="23"/>
-      <c r="Y7" s="24"/>
-      <c r="Z7" s="23"/>
-      <c r="AA7" s="24"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="24"/>
-      <c r="AD7" s="23"/>
-      <c r="AE7" s="24"/>
-      <c r="AF7" s="23"/>
-      <c r="AG7" s="24"/>
-      <c r="AH7" s="23"/>
-      <c r="AI7" s="24"/>
-      <c r="AJ7" s="23"/>
-      <c r="AK7" s="24"/>
-      <c r="AL7" s="23"/>
-      <c r="AM7" s="24"/>
-      <c r="AN7" s="23"/>
-      <c r="AO7" s="24"/>
-      <c r="AP7" s="23"/>
-      <c r="AQ7" s="24"/>
-      <c r="AR7" s="23"/>
-      <c r="AS7" s="24"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="26"/>
+      <c r="X7" s="25"/>
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="25"/>
+      <c r="AA7" s="26"/>
+      <c r="AB7" s="25"/>
+      <c r="AC7" s="26"/>
+      <c r="AD7" s="25"/>
+      <c r="AE7" s="26"/>
+      <c r="AF7" s="25"/>
+      <c r="AG7" s="26"/>
+      <c r="AH7" s="25"/>
+      <c r="AI7" s="26"/>
+      <c r="AJ7" s="25"/>
+      <c r="AK7" s="26"/>
+      <c r="AL7" s="25"/>
+      <c r="AM7" s="26"/>
+      <c r="AN7" s="25"/>
+      <c r="AO7" s="26"/>
+      <c r="AP7" s="25"/>
+      <c r="AQ7" s="26"/>
+      <c r="AR7" s="25"/>
+      <c r="AS7" s="26"/>
       <c r="AT7" s="21"/>
       <c r="AU7" s="10"/>
     </row>
-    <row r="8" spans="1:47" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:47" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="20"/>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C8" s="4">
-        <v>45011</v>
+        <v>45006</v>
       </c>
       <c r="D8" s="4">
-        <v>45022</v>
+        <v>45008</v>
       </c>
       <c r="E8" s="3">
-        <v>4</v>
-      </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="24"/>
-      <c r="AD8" s="23"/>
-      <c r="AE8" s="24"/>
-      <c r="AF8" s="23"/>
-      <c r="AG8" s="24"/>
-      <c r="AH8" s="23"/>
-      <c r="AI8" s="24"/>
-      <c r="AJ8" s="23"/>
-      <c r="AK8" s="24"/>
-      <c r="AL8" s="23"/>
-      <c r="AM8" s="24"/>
-      <c r="AN8" s="23"/>
-      <c r="AO8" s="24"/>
-      <c r="AP8" s="23"/>
-      <c r="AQ8" s="24"/>
-      <c r="AR8" s="23"/>
-      <c r="AS8" s="24"/>
+        <v>2</v>
+      </c>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="26"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="26"/>
+      <c r="X8" s="25"/>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="25"/>
+      <c r="AA8" s="26"/>
+      <c r="AB8" s="25"/>
+      <c r="AC8" s="26"/>
+      <c r="AD8" s="25"/>
+      <c r="AE8" s="26"/>
+      <c r="AF8" s="25"/>
+      <c r="AG8" s="26"/>
+      <c r="AH8" s="25"/>
+      <c r="AI8" s="26"/>
+      <c r="AJ8" s="25"/>
+      <c r="AK8" s="26"/>
+      <c r="AL8" s="25"/>
+      <c r="AM8" s="26"/>
+      <c r="AN8" s="25"/>
+      <c r="AO8" s="26"/>
+      <c r="AP8" s="25"/>
+      <c r="AQ8" s="26"/>
+      <c r="AR8" s="25"/>
+      <c r="AS8" s="26"/>
       <c r="AT8" s="21"/>
       <c r="AU8" s="10"/>
     </row>
-    <row r="9" spans="1:47" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:47" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="20"/>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C9" s="4">
-        <v>45021</v>
+        <v>45011</v>
       </c>
       <c r="D9" s="4">
-        <v>45031</v>
+        <v>45022</v>
       </c>
       <c r="E9" s="3">
-        <v>3</v>
-      </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="24"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="24"/>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="24"/>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="24"/>
-      <c r="AD9" s="23"/>
-      <c r="AE9" s="24"/>
-      <c r="AF9" s="23"/>
-      <c r="AG9" s="24"/>
-      <c r="AH9" s="23"/>
-      <c r="AI9" s="24"/>
-      <c r="AJ9" s="23"/>
-      <c r="AK9" s="24"/>
-      <c r="AL9" s="23"/>
-      <c r="AM9" s="24"/>
-      <c r="AN9" s="23"/>
-      <c r="AO9" s="24"/>
-      <c r="AP9" s="23"/>
-      <c r="AQ9" s="24"/>
-      <c r="AR9" s="23"/>
-      <c r="AS9" s="24"/>
+        <v>4</v>
+      </c>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="26"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="25"/>
+      <c r="AA9" s="26"/>
+      <c r="AB9" s="25"/>
+      <c r="AC9" s="26"/>
+      <c r="AD9" s="25"/>
+      <c r="AE9" s="26"/>
+      <c r="AF9" s="25"/>
+      <c r="AG9" s="26"/>
+      <c r="AH9" s="25"/>
+      <c r="AI9" s="26"/>
+      <c r="AJ9" s="25"/>
+      <c r="AK9" s="26"/>
+      <c r="AL9" s="25"/>
+      <c r="AM9" s="26"/>
+      <c r="AN9" s="25"/>
+      <c r="AO9" s="26"/>
+      <c r="AP9" s="25"/>
+      <c r="AQ9" s="26"/>
+      <c r="AR9" s="25"/>
+      <c r="AS9" s="26"/>
       <c r="AT9" s="21"/>
       <c r="AU9" s="10"/>
     </row>
-    <row r="10" spans="1:47" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:47" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="20"/>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C10" s="4">
-        <v>45025</v>
+        <v>45021</v>
       </c>
       <c r="D10" s="4">
-        <v>45036</v>
+        <v>45031</v>
       </c>
       <c r="E10" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -3914,19 +4045,19 @@
       <c r="AT10" s="21"/>
       <c r="AU10" s="10"/>
     </row>
-    <row r="11" spans="1:47" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:47" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="20"/>
       <c r="B11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="9">
-        <v>45032</v>
-      </c>
-      <c r="D11" s="9">
-        <v>45059</v>
+        <v>12</v>
+      </c>
+      <c r="C11" s="4">
+        <v>45025</v>
+      </c>
+      <c r="D11" s="4">
+        <v>45036</v>
       </c>
       <c r="E11" s="3">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -3971,19 +4102,19 @@
       <c r="AT11" s="21"/>
       <c r="AU11" s="10"/>
     </row>
-    <row r="12" spans="1:47" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:47" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="20"/>
       <c r="B12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="4">
-        <v>45046</v>
-      </c>
-      <c r="D12" s="4">
-        <v>45057</v>
+        <v>17</v>
+      </c>
+      <c r="C12" s="9">
+        <v>45032</v>
+      </c>
+      <c r="D12" s="9">
+        <v>45059</v>
       </c>
       <c r="E12" s="3">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -4028,19 +4159,19 @@
       <c r="AT12" s="21"/>
       <c r="AU12" s="10"/>
     </row>
-    <row r="13" spans="1:47" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:47" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="20"/>
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C13" s="4">
-        <v>45060</v>
+        <v>45046</v>
       </c>
       <c r="D13" s="4">
-        <v>45084</v>
+        <v>45057</v>
       </c>
       <c r="E13" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -4084,19 +4215,19 @@
       <c r="AS13" s="24"/>
       <c r="AT13" s="20"/>
     </row>
-    <row r="14" spans="1:47" ht="64" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:47" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="20"/>
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="4">
-        <v>45081</v>
+        <v>45060</v>
       </c>
       <c r="D14" s="4">
-        <v>45094</v>
-      </c>
-      <c r="E14" s="8">
-        <v>6</v>
+        <v>45084</v>
+      </c>
+      <c r="E14" s="3">
+        <v>10</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -4140,15 +4271,15 @@
       <c r="AS14" s="24"/>
       <c r="AT14" s="20"/>
     </row>
-    <row r="15" spans="1:47" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="22">
-        <v>45088</v>
-      </c>
-      <c r="D15" s="22">
-        <v>45101</v>
+    <row r="15" spans="1:47" ht="64" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="4">
+        <v>45081</v>
+      </c>
+      <c r="D15" s="4">
+        <v>45094</v>
       </c>
       <c r="E15" s="8">
         <v>6</v>
@@ -4195,19 +4326,19 @@
       <c r="AS15" s="24"/>
       <c r="AT15" s="20"/>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:47" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
-      <c r="B16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="4">
-        <v>45092</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="B16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="22">
+        <v>45088</v>
+      </c>
+      <c r="D16" s="22">
         <v>45101</v>
       </c>
-      <c r="E16" s="3">
-        <v>3</v>
+      <c r="E16" s="8">
+        <v>6</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -4252,266 +4383,307 @@
       <c r="AT16" s="20"/>
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="12">
-        <v>5</v>
-      </c>
-      <c r="G17" s="13">
-        <v>11</v>
-      </c>
-      <c r="H17" s="12">
-        <v>12</v>
-      </c>
-      <c r="I17" s="13">
-        <v>18</v>
-      </c>
-      <c r="J17" s="12">
-        <v>19</v>
-      </c>
-      <c r="K17" s="13">
-        <v>25</v>
-      </c>
-      <c r="L17" s="12">
-        <v>26</v>
-      </c>
-      <c r="M17" s="13">
-        <v>4</v>
-      </c>
-      <c r="N17" s="12">
-        <v>5</v>
-      </c>
-      <c r="O17" s="13">
-        <v>11</v>
-      </c>
-      <c r="P17" s="12">
-        <v>12</v>
-      </c>
-      <c r="Q17" s="13">
-        <v>18</v>
-      </c>
-      <c r="R17" s="12">
-        <v>19</v>
-      </c>
-      <c r="S17" s="13">
-        <v>25</v>
-      </c>
-      <c r="T17" s="12">
-        <v>26</v>
-      </c>
-      <c r="U17" s="13">
-        <v>1</v>
-      </c>
-      <c r="V17" s="12">
-        <v>2</v>
-      </c>
-      <c r="W17" s="13">
+      <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="X17" s="12">
-        <v>9</v>
-      </c>
-      <c r="Y17" s="13">
-        <v>15</v>
-      </c>
-      <c r="Z17" s="12">
-        <v>16</v>
-      </c>
-      <c r="AA17" s="13">
-        <v>22</v>
-      </c>
-      <c r="AB17" s="12">
-        <v>23</v>
-      </c>
-      <c r="AC17" s="13">
-        <v>29</v>
-      </c>
-      <c r="AD17" s="12">
-        <v>30</v>
-      </c>
-      <c r="AE17" s="13">
-        <v>6</v>
-      </c>
-      <c r="AF17" s="12">
-        <v>7</v>
-      </c>
-      <c r="AG17" s="13">
-        <v>13</v>
-      </c>
-      <c r="AH17" s="12">
-        <v>14</v>
-      </c>
-      <c r="AI17" s="13">
-        <v>20</v>
-      </c>
-      <c r="AJ17" s="12">
-        <v>21</v>
-      </c>
-      <c r="AK17" s="13">
-        <v>27</v>
-      </c>
-      <c r="AL17" s="12">
-        <v>28</v>
-      </c>
-      <c r="AM17" s="13">
+      <c r="C17" s="4">
+        <v>45092</v>
+      </c>
+      <c r="D17" s="4">
+        <v>45101</v>
+      </c>
+      <c r="E17" s="3">
         <v>3</v>
       </c>
-      <c r="AN17" s="12">
-        <v>4</v>
-      </c>
-      <c r="AO17" s="13">
-        <v>10</v>
-      </c>
-      <c r="AP17" s="12">
-        <v>11</v>
-      </c>
-      <c r="AQ17" s="13">
-        <v>17</v>
-      </c>
-      <c r="AR17" s="12">
-        <v>18</v>
-      </c>
-      <c r="AS17" s="13">
-        <v>24</v>
-      </c>
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="23"/>
+      <c r="Y17" s="24"/>
+      <c r="Z17" s="23"/>
+      <c r="AA17" s="24"/>
+      <c r="AB17" s="23"/>
+      <c r="AC17" s="24"/>
+      <c r="AD17" s="23"/>
+      <c r="AE17" s="24"/>
+      <c r="AF17" s="23"/>
+      <c r="AG17" s="24"/>
+      <c r="AH17" s="23"/>
+      <c r="AI17" s="24"/>
+      <c r="AJ17" s="23"/>
+      <c r="AK17" s="24"/>
+      <c r="AL17" s="23"/>
+      <c r="AM17" s="24"/>
+      <c r="AN17" s="23"/>
+      <c r="AO17" s="24"/>
+      <c r="AP17" s="23"/>
+      <c r="AQ17" s="24"/>
+      <c r="AR17" s="23"/>
+      <c r="AS17" s="24"/>
       <c r="AT17" s="20"/>
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="2" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="12">
+        <v>5</v>
+      </c>
+      <c r="G18" s="13">
+        <v>11</v>
+      </c>
+      <c r="H18" s="12">
+        <v>12</v>
+      </c>
+      <c r="I18" s="13">
+        <v>18</v>
+      </c>
+      <c r="J18" s="12">
+        <v>19</v>
+      </c>
+      <c r="K18" s="13">
+        <v>25</v>
+      </c>
+      <c r="L18" s="12">
+        <v>26</v>
+      </c>
+      <c r="M18" s="13">
+        <v>4</v>
+      </c>
+      <c r="N18" s="12">
+        <v>5</v>
+      </c>
+      <c r="O18" s="13">
+        <v>11</v>
+      </c>
+      <c r="P18" s="12">
+        <v>12</v>
+      </c>
+      <c r="Q18" s="13">
+        <v>18</v>
+      </c>
+      <c r="R18" s="12">
+        <v>19</v>
+      </c>
+      <c r="S18" s="13">
+        <v>25</v>
+      </c>
+      <c r="T18" s="12">
+        <v>26</v>
+      </c>
+      <c r="U18" s="13">
+        <v>1</v>
+      </c>
+      <c r="V18" s="12">
+        <v>2</v>
+      </c>
+      <c r="W18" s="13">
+        <v>8</v>
+      </c>
+      <c r="X18" s="12">
+        <v>9</v>
+      </c>
+      <c r="Y18" s="13">
+        <v>15</v>
+      </c>
+      <c r="Z18" s="12">
+        <v>16</v>
+      </c>
+      <c r="AA18" s="13">
+        <v>22</v>
+      </c>
+      <c r="AB18" s="12">
+        <v>23</v>
+      </c>
+      <c r="AC18" s="13">
+        <v>29</v>
+      </c>
+      <c r="AD18" s="12">
+        <v>30</v>
+      </c>
+      <c r="AE18" s="13">
         <v>6</v>
       </c>
-      <c r="F18" s="33">
-        <v>2</v>
-      </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="33">
+      <c r="AF18" s="12">
+        <v>7</v>
+      </c>
+      <c r="AG18" s="13">
+        <v>13</v>
+      </c>
+      <c r="AH18" s="12">
+        <v>14</v>
+      </c>
+      <c r="AI18" s="13">
+        <v>20</v>
+      </c>
+      <c r="AJ18" s="12">
+        <v>21</v>
+      </c>
+      <c r="AK18" s="13">
+        <v>27</v>
+      </c>
+      <c r="AL18" s="12">
+        <v>28</v>
+      </c>
+      <c r="AM18" s="13">
         <v>3</v>
       </c>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="34"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="33">
+      <c r="AN18" s="12">
         <v>4</v>
       </c>
-      <c r="V18" s="34"/>
-      <c r="W18" s="34"/>
-      <c r="X18" s="34"/>
-      <c r="Y18" s="34"/>
-      <c r="Z18" s="34"/>
-      <c r="AA18" s="34"/>
-      <c r="AB18" s="34"/>
-      <c r="AC18" s="34"/>
-      <c r="AD18" s="35"/>
-      <c r="AE18" s="33">
-        <v>5</v>
-      </c>
-      <c r="AF18" s="34"/>
-      <c r="AG18" s="34"/>
-      <c r="AH18" s="34"/>
-      <c r="AI18" s="34"/>
-      <c r="AJ18" s="34"/>
-      <c r="AK18" s="34"/>
-      <c r="AL18" s="35"/>
-      <c r="AM18" s="33">
-        <v>6</v>
-      </c>
-      <c r="AN18" s="34"/>
-      <c r="AO18" s="34"/>
-      <c r="AP18" s="34"/>
-      <c r="AQ18" s="34"/>
-      <c r="AR18" s="34"/>
-      <c r="AS18" s="35"/>
+      <c r="AO18" s="13">
+        <v>10</v>
+      </c>
+      <c r="AP18" s="12">
+        <v>11</v>
+      </c>
+      <c r="AQ18" s="13">
+        <v>17</v>
+      </c>
+      <c r="AR18" s="12">
+        <v>18</v>
+      </c>
+      <c r="AS18" s="13">
+        <v>24</v>
+      </c>
       <c r="AT18" s="20"/>
     </row>
     <row r="19" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="20"/>
-      <c r="U19" s="20"/>
-      <c r="V19" s="20"/>
-      <c r="W19" s="20"/>
-      <c r="X19" s="20"/>
-      <c r="Y19" s="20"/>
-      <c r="Z19" s="20"/>
-      <c r="AA19" s="20"/>
-      <c r="AB19" s="20"/>
-      <c r="AC19" s="20"/>
-      <c r="AD19" s="20"/>
-      <c r="AE19" s="20"/>
-      <c r="AF19" s="20"/>
-      <c r="AG19" s="20"/>
-      <c r="AH19" s="20"/>
-      <c r="AI19" s="20"/>
-      <c r="AJ19" s="20"/>
-      <c r="AK19" s="20"/>
-      <c r="AL19" s="20"/>
-      <c r="AM19" s="20"/>
-      <c r="AN19" s="20"/>
-      <c r="AO19" s="20"/>
-      <c r="AP19" s="20"/>
-      <c r="AQ19" s="20"/>
-      <c r="AR19" s="20"/>
-      <c r="AS19" s="20"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="35">
+        <v>2</v>
+      </c>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="35">
+        <v>3</v>
+      </c>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="37"/>
+      <c r="U19" s="35">
+        <v>4</v>
+      </c>
+      <c r="V19" s="36"/>
+      <c r="W19" s="36"/>
+      <c r="X19" s="36"/>
+      <c r="Y19" s="36"/>
+      <c r="Z19" s="36"/>
+      <c r="AA19" s="36"/>
+      <c r="AB19" s="36"/>
+      <c r="AC19" s="36"/>
+      <c r="AD19" s="37"/>
+      <c r="AE19" s="35">
+        <v>5</v>
+      </c>
+      <c r="AF19" s="36"/>
+      <c r="AG19" s="36"/>
+      <c r="AH19" s="36"/>
+      <c r="AI19" s="36"/>
+      <c r="AJ19" s="36"/>
+      <c r="AK19" s="36"/>
+      <c r="AL19" s="37"/>
+      <c r="AM19" s="35">
+        <v>6</v>
+      </c>
+      <c r="AN19" s="36"/>
+      <c r="AO19" s="36"/>
+      <c r="AP19" s="36"/>
+      <c r="AQ19" s="36"/>
+      <c r="AR19" s="36"/>
+      <c r="AS19" s="37"/>
       <c r="AT19" s="20"/>
     </row>
+    <row r="20" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="20"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="20"/>
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="20"/>
+      <c r="AB20" s="20"/>
+      <c r="AC20" s="20"/>
+      <c r="AD20" s="20"/>
+      <c r="AE20" s="20"/>
+      <c r="AF20" s="20"/>
+      <c r="AG20" s="20"/>
+      <c r="AH20" s="20"/>
+      <c r="AI20" s="20"/>
+      <c r="AJ20" s="20"/>
+      <c r="AK20" s="20"/>
+      <c r="AL20" s="20"/>
+      <c r="AM20" s="20"/>
+      <c r="AN20" s="20"/>
+      <c r="AO20" s="20"/>
+      <c r="AP20" s="20"/>
+      <c r="AQ20" s="20"/>
+      <c r="AR20" s="20"/>
+      <c r="AS20" s="20"/>
+      <c r="AT20" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="290">
-    <mergeCell ref="AP7:AQ7"/>
-    <mergeCell ref="AR7:AS7"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="AD7:AE7"/>
-    <mergeCell ref="AF7:AG7"/>
-    <mergeCell ref="AH7:AI7"/>
-    <mergeCell ref="AJ7:AK7"/>
-    <mergeCell ref="AL7:AM7"/>
-    <mergeCell ref="AN7:AO7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="AP16:AQ16"/>
-    <mergeCell ref="AR16:AS16"/>
+  <mergeCells count="150">
+    <mergeCell ref="F19:L19"/>
+    <mergeCell ref="M19:T19"/>
+    <mergeCell ref="U19:AD19"/>
+    <mergeCell ref="AE19:AL19"/>
+    <mergeCell ref="AM19:AS19"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="F2:AS2"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
@@ -4531,187 +4703,43 @@
     <mergeCell ref="AL8:AM8"/>
     <mergeCell ref="AN8:AO8"/>
     <mergeCell ref="AP8:AQ8"/>
-    <mergeCell ref="AR8:AS8"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AD16:AE16"/>
-    <mergeCell ref="AF16:AG16"/>
-    <mergeCell ref="AH16:AI16"/>
-    <mergeCell ref="AJ16:AK16"/>
-    <mergeCell ref="AL16:AM16"/>
-    <mergeCell ref="AN16:AO16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="AP14:AQ14"/>
-    <mergeCell ref="AR14:AS14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="T15:U15"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="X15:Y15"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AD15:AE15"/>
-    <mergeCell ref="AF15:AG15"/>
-    <mergeCell ref="AH15:AI15"/>
-    <mergeCell ref="AJ15:AK15"/>
-    <mergeCell ref="AL15:AM15"/>
-    <mergeCell ref="AN15:AO15"/>
-    <mergeCell ref="AP15:AQ15"/>
-    <mergeCell ref="AR15:AS15"/>
-    <mergeCell ref="X14:Y14"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AD14:AE14"/>
-    <mergeCell ref="AF14:AG14"/>
-    <mergeCell ref="AH14:AI14"/>
-    <mergeCell ref="AJ14:AK14"/>
-    <mergeCell ref="AL14:AM14"/>
-    <mergeCell ref="AN14:AO14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="AP12:AQ12"/>
-    <mergeCell ref="AR12:AS12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="AF13:AG13"/>
-    <mergeCell ref="AH13:AI13"/>
-    <mergeCell ref="AJ13:AK13"/>
-    <mergeCell ref="AL13:AM13"/>
-    <mergeCell ref="AN13:AO13"/>
-    <mergeCell ref="AP13:AQ13"/>
-    <mergeCell ref="AR13:AS13"/>
-    <mergeCell ref="X12:Y12"/>
-    <mergeCell ref="Z12:AA12"/>
-    <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="AD12:AE12"/>
-    <mergeCell ref="AF12:AG12"/>
-    <mergeCell ref="AH12:AI12"/>
-    <mergeCell ref="AJ12:AK12"/>
-    <mergeCell ref="AL12:AM12"/>
-    <mergeCell ref="AN12:AO12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="T12:U12"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="AJ9:AK9"/>
-    <mergeCell ref="AL9:AM9"/>
-    <mergeCell ref="AN9:AO9"/>
-    <mergeCell ref="AP9:AQ9"/>
-    <mergeCell ref="AR9:AS9"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="T11:U11"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="X11:Y11"/>
-    <mergeCell ref="Z11:AA11"/>
-    <mergeCell ref="AB11:AC11"/>
-    <mergeCell ref="AD11:AE11"/>
-    <mergeCell ref="AF11:AG11"/>
-    <mergeCell ref="AH11:AI11"/>
-    <mergeCell ref="AJ11:AK11"/>
-    <mergeCell ref="AL11:AM11"/>
-    <mergeCell ref="AN11:AO11"/>
-    <mergeCell ref="AP11:AQ11"/>
-    <mergeCell ref="AR11:AS11"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="X9:Y9"/>
-    <mergeCell ref="Z9:AA9"/>
-    <mergeCell ref="AB9:AC9"/>
-    <mergeCell ref="AD9:AE9"/>
-    <mergeCell ref="AF9:AG9"/>
-    <mergeCell ref="AH9:AI9"/>
-    <mergeCell ref="F18:L18"/>
-    <mergeCell ref="M18:T18"/>
-    <mergeCell ref="U18:AD18"/>
-    <mergeCell ref="AE18:AL18"/>
-    <mergeCell ref="AM18:AS18"/>
-    <mergeCell ref="AJ6:AK6"/>
-    <mergeCell ref="AL6:AM6"/>
-    <mergeCell ref="T10:U10"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="X10:Y10"/>
-    <mergeCell ref="Z10:AA10"/>
-    <mergeCell ref="AB10:AC10"/>
-    <mergeCell ref="AD10:AE10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="AH5:AI5"/>
-    <mergeCell ref="AJ5:AK5"/>
-    <mergeCell ref="AL5:AM5"/>
-    <mergeCell ref="AN5:AO5"/>
-    <mergeCell ref="AP5:AQ5"/>
-    <mergeCell ref="AR5:AS5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="AN6:AO6"/>
-    <mergeCell ref="AP6:AQ6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="AR6:AS6"/>
-    <mergeCell ref="AF6:AG6"/>
-    <mergeCell ref="AH6:AI6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AR3:AS3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AH4:AI4"/>
+    <mergeCell ref="N3:O3"/>
     <mergeCell ref="Z3:AA3"/>
     <mergeCell ref="AP4:AQ4"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="R10:S10"/>
     <mergeCell ref="AJ4:AK4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="AN4:AO4"/>
@@ -4732,57 +4760,76 @@
     <mergeCell ref="AD5:AE5"/>
     <mergeCell ref="AF5:AG5"/>
     <mergeCell ref="V6:W6"/>
-    <mergeCell ref="AJ10:AK10"/>
-    <mergeCell ref="AL10:AM10"/>
+    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="AL5:AM5"/>
+    <mergeCell ref="AN5:AO5"/>
+    <mergeCell ref="AP5:AQ5"/>
+    <mergeCell ref="AR5:AS5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="AJ6:AK6"/>
+    <mergeCell ref="AL6:AM6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="AN6:AO6"/>
+    <mergeCell ref="AP6:AQ6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="AR6:AS6"/>
+    <mergeCell ref="AF6:AG6"/>
+    <mergeCell ref="AH6:AI6"/>
     <mergeCell ref="AB6:AC6"/>
     <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="AR3:AS3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="AN10:AO10"/>
-    <mergeCell ref="AP10:AQ10"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AH4:AI4"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="F2:AS2"/>
-    <mergeCell ref="AR10:AS10"/>
-    <mergeCell ref="AF10:AG10"/>
-    <mergeCell ref="AH10:AI10"/>
+    <mergeCell ref="AR8:AS8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="Z9:AA9"/>
+    <mergeCell ref="AB9:AC9"/>
+    <mergeCell ref="AD9:AE9"/>
+    <mergeCell ref="AF9:AG9"/>
+    <mergeCell ref="AH9:AI9"/>
+    <mergeCell ref="AJ9:AK9"/>
+    <mergeCell ref="AL9:AM9"/>
+    <mergeCell ref="AN9:AO9"/>
+    <mergeCell ref="AP9:AQ9"/>
+    <mergeCell ref="AR9:AS9"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="AP7:AQ7"/>
+    <mergeCell ref="AR7:AS7"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="AF7:AG7"/>
+    <mergeCell ref="AH7:AI7"/>
+    <mergeCell ref="AJ7:AK7"/>
+    <mergeCell ref="AL7:AM7"/>
+    <mergeCell ref="AN7:AO7"/>
   </mergeCells>
-  <conditionalFormatting sqref="F4:F16 H4:H16 J4:J16 L4:L16 N4:N16 P4:P16 R4:R16 T4:T16 V4:V16 X4:X16 Z4:Z16 AB4:AB16 AD4:AD16 AF4:AF16 AH4:AH16 AJ4:AJ16 AL4:AL16 AN4:AN16 AP4:AP16 AR4:AR16">
-    <cfRule type="dataBar" priority="58">
+  <conditionalFormatting sqref="F4:F17 H4:H17 J4:J17 L4:L17 N4:N17 P4:P17 R4:R17 T4:T17 V4:V17 X4:X17 Z4:Z17 AB4:AB17 AD4:AD17 AF4:AF17 AH4:AH17 AJ4:AJ17 AL4:AL17 AN4:AN17 AP4:AP17 AR4:AR17">
+    <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4809,7 +4856,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F4:F16 H4:H16 J4:J16 L4:L16 N4:N16 P4:P16 R4:R16 T4:T16 V4:V16 X4:X16 Z4:Z16 AB4:AB16 AD4:AD16 AF4:AF16 AH4:AH16 AJ4:AJ16 AL4:AL16 AN4:AN16 AP4:AP16 AR4:AR16</xm:sqref>
+          <xm:sqref>F4:F17 H4:H17 J4:J17 L4:L17 N4:N17 P4:P17 R4:R17 T4:T17 V4:V17 X4:X17 Z4:Z17 AB4:AB17 AD4:AD17 AF4:AF17 AH4:AH17 AJ4:AJ17 AL4:AL17 AN4:AN17 AP4:AP17 AR4:AR17</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>